<commit_message>
Fix: Backend plan reset logic and Mobile App date sync
</commit_message>
<xml_diff>
--- a/backend/Coordinados (11).xlsx
+++ b/backend/Coordinados (11).xlsx
@@ -8,22 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{6E90B41F-D867-42A0-807A-512850833FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0765AED5-5002-483F-96E0-3FAA4AC360C3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA37CA90-A6B0-485F-BA68-006FFD55D342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{8EB25C48-5E99-49DF-854C-F5A7791473A5}"/>
+    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{F9CA0F41-2E70-4754-8728-A810F4F5D8DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coordinados!$A$1:$BG$17</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="144">
   <si>
     <t>ID</t>
   </si>
@@ -226,286 +223,388 @@
     <t>abierta</t>
   </si>
   <si>
-    <t>26-12-2025</t>
-  </si>
-  <si>
     <t>público</t>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
-    <t>83614800-2</t>
-  </si>
-  <si>
     <t>Arriendo</t>
   </si>
   <si>
-    <t>Cámara</t>
-  </si>
-  <si>
     <t>Soporte</t>
   </si>
   <si>
     <t>18-12-2025</t>
   </si>
   <si>
-    <t>TALAGANTE - SOPORTE GPS - MONTINA - MONTINA_CAMARA4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad: REVISION DE GPS 
-Accesorio: SONDA DE T°  
-subcuenta visualización: FLOTA_MONTINA 
-Año GPS: 2024 
-Observación: UNIDAD CON SONDA DE T° PEGADA. FAVOR COORDINAR VISITA TENICA  
+    <t>GV310LAU</t>
+  </si>
+  <si>
+    <t>Región Metropolitana de Santiago.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soporte</t>
+  </si>
+  <si>
+    <t>Blanca Acuña</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>Antena GPS</t>
+  </si>
+  <si>
+    <t>Vehículo</t>
+  </si>
+  <si>
+    <t>CIAL_ALIMENTOS</t>
+  </si>
+  <si>
+    <t>80186300-0</t>
+  </si>
+  <si>
+    <t>Camión</t>
+  </si>
+  <si>
+    <t>Instalación</t>
+  </si>
+  <si>
+    <t>AMERICO VESPUCIO 2341 PUDAHUEL</t>
+  </si>
+  <si>
+    <t>PUDAHUEL</t>
+  </si>
+  <si>
+    <t>VICTOR JIMENEZ</t>
+  </si>
+  <si>
+    <t>nicolas.zuniga@cial.cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDACIÓN I+D  
+1.- VALIDAR POSICION DE DISPOSITIVO GPS  
+2.- VALIDACIÓN DE FUNCIONAMIENTO BOTON EMERGENCIA  
+3.- VALIDACIÓN DE FUNCIONAMIENTO CORTE MOTOR  
+4.- VALIDACIÓN DE FUNCIONAMIENTO SENSOR PUERTA  
+5.- VALIDACIÓN DE SENSOR DE TEMPERATURA (AMBAS SONDAS DEBEN ESTAR FUNCIONALES) 
+6.- FOTOGRAFIA DE GPS COMPETENCIA (NUMERO DE SERIE)  
+7.- FOTOGRAFÍA FISICA DE LA UBICACIÓN DEL GPS (DONDE QUEDA INSTALADO) (OBLIGATORIO) 
+8.- FOTOGRAFÍA DE PATENTE INTERVENIDA  
+9.- OT FIRMADA  
+10.- DAR VISUALIZACIÓN A SUBCUENTA FLOTA_CIALALIMENTOS 
+ZONA Y ALARMA  
+1.- VELOCIDAD 95 KM POR 1 MINUTO  
+2.- CARGA DE ZONAS POR ACCESORIOS IMPLEMENTADOS  
+3.- CARGAR ALARMA DE TEMPERATURA PEGADA  
+4.- SIN COBERTURA GPS  
 </t>
   </si>
   <si>
-    <t xml:space="preserve">@Soledad Brito 26-12-2025 16:09
-COORDINADO CON LUIS ZUÑIGA PARA 29.12.25 A LAS 10:00 HRS.
-</t>
-  </si>
-  <si>
-    <t>ARIZSANTIAGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104124 </t>
-  </si>
-  <si>
-    <t>MONTINA_CAMARA4</t>
-  </si>
-  <si>
-    <t>GV310LAU</t>
-  </si>
-  <si>
-    <t>lzuniga@ariztia.com</t>
-  </si>
-  <si>
-    <t>LUIS ZUÑIGA</t>
-  </si>
-  <si>
-    <t>Bernardo Ohiggins 0128, Talagante</t>
-  </si>
-  <si>
-    <t>TALAGANTE</t>
-  </si>
-  <si>
-    <t>Región Metropolitana de Santiago.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Soporte</t>
-  </si>
-  <si>
-    <t>Blanca Acuña</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>Antena GPS</t>
-  </si>
-  <si>
-    <t>urgente</t>
-  </si>
-  <si>
-    <t>CIAL_ALIMENTOS</t>
-  </si>
-  <si>
-    <t>80186300-0</t>
-  </si>
-  <si>
-    <t>Camión</t>
-  </si>
-  <si>
-    <t>22-12-2025</t>
-  </si>
-  <si>
-    <t>Joaquin Lopez</t>
-  </si>
-  <si>
-    <t>asignada</t>
-  </si>
-  <si>
-    <t>reabierta</t>
-  </si>
-  <si>
-    <t>CERRILLOS - SOPORTE GPS - ARIZSANTIAGO - CDPO-3905-LCHD38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad: REVISION DE GPS  
-Accesorio: ANTENA GPS, BOTÓN ALÁMBRICO TABLERO, CORTA CORRIENTE REMOTO, SENSOR PUERTA, SENSOR TEMPERATURA 
-subcuenta visualización: FLOTA_ARIZSANTIAGO 
-Año GPS: 2025 
-Marca: HINO 
-Modelo: XZU 
-Año: 2019 
-Observación: UNIDAD REGISTRA DATOS DE T! PEGADA. FAVOR COORDINAR Y REALIZAR VISITA TECNICA.  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 26-12-2025 11:47
-RECOORDINADO CON CRISTIAN DELGADO PARA 29.12.25 A LAS 16:00 HRS.
-=-=
-@José Cabrera 26-12-2025 10:22
-Estimados, comento que unidad volvio a fallar y la T° aun continua pegada.  
-Favor volver a revisar en terreno de forma urgente.
-=-=
-@Joaquin Lopez 22-12-2025 19:29
-CAMBIO DE SONDA, CAMBIO DE GPS ENTEL A MANAGER
-=-=
-@Soledad Brito 22-12-2025 15:25
-COORDINADO CON CRISTIAN DELGADO PARA 22.12.25 A LAS 18:30 HRS.
-</t>
-  </si>
-  <si>
-    <t>61701</t>
-  </si>
-  <si>
-    <t>CDPO-3905-LCHD38</t>
-  </si>
-  <si>
-    <t>cdelgadob@ariztia.com</t>
-  </si>
-  <si>
-    <t>CRISTIAN DELGADO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VISTA ALEGRE NRO. 2350, CERRILLOS </t>
-  </si>
-  <si>
-    <t>CERRILLOS</t>
-  </si>
-  <si>
-    <t>Cambio de accesorios</t>
-  </si>
-  <si>
-    <t>23-12-2025</t>
-  </si>
-  <si>
-    <t>SANTIAGO - REVISION GPS - CIAL_ALIMENTOS - VE103-HCDX49</t>
-  </si>
-  <si>
-    <t>ACTIVIDAD : REVISION GPS SIN TRANSMITIR SE CONFIRMA UNIDAD EN RUTA Y ENVIO DE COMANDOS RESERT 
-Información vehicular 
-Patente HCDX49-5 
-Tipo CAMION 
-Marca HINO 
-Modelo XZU CITY 
-Año 2015 
-Color BLANCO 
-N° Motor N04C VC11024 
-N° Chasis JHHACN4H0FK002219 
-Procedencia JAPAN 
-Fabricante HINO 
-Tipo de sello SELLO VERDE 
-Combustible DIESEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I+D 
-COMENTARIOS DETALLES DE ACTIVIDAD REALIZADA 
-VALIDACIÓN 
-1.- VALIDAR POSICION DE DISPOSITIVO GPS 
-2.- VALIDACIÓN DE FUNCIONAMIENTO BOTON EMERGENCIA 
-3.- VALIDACIÓN DE FUNCIONAMIENTO CORTE MOTOR 
-4.- VALIDACIÓN DE FUNCIONAMIENTO SENSOR PUERTA 
-5.- VALIDACIÓN DE SENSOR DE TEMPERATURA (AMBAS SONDAS DEBEN ESTAR FUNCIONALES) 
-6.- FOTOGRAFÍA DE PATENTE INTERVENIDA 
-9.- OT FIRMADA 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 26-12-2025 10:28
-COORDINADO CON EDUARDO PARA 05.01.25 A LAS 10:00 HRS.
-</t>
-  </si>
-  <si>
-    <t>114579</t>
-  </si>
-  <si>
-    <t>VE103-HCDX49</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Revisión</t>
-  </si>
-  <si>
-    <t>EDUARDO  ORTIZ</t>
-  </si>
-  <si>
-    <t>AMERICO VESPUCIO 2341 PUDAHUEL</t>
-  </si>
-  <si>
-    <t>PUDAHUEL</t>
-  </si>
-  <si>
-    <t>10-12-2025</t>
-  </si>
-  <si>
-    <t>SANTIAGO - REVISION GPS + ACCESORIOS - CIAL_ALIMENTOS - PRSV10</t>
-  </si>
-  <si>
-    <t>ACTIVIDAD: REVISIÓN GPS + CORTE DE MOTOR 
-CLIENTE INDICA QUE DESDE INSTALACIÓN UNIDAD PRESENTA PROBLEMA EN SU PANEL, TENIENDO LUCES INTERMITENTES Y EL DIA DE HOY 10-12 A LAS 08:48:53 POSTERIOR A TERMINAR UN ENTREGA ENCENDIO LA UNIDAD SIN EXITO, SE ENVIARON COMANDOS SIN EXITO A TRAVES DE PLATAFORMA NO SE OBSERVABA CORTE DE MOTOR, CLIENTE ACUDIO A TECNICO ELECTRICITA EL CUAL DESCONEXTO LA UNIDAD Y LOGRO ENCENDER. 
- ACTIVIDAD: VALIDACION DE INSTALACION 
-GPS 
-BOTON EMERGENCIA 
-CORTE MOTOR 
+    <t xml:space="preserve">Instalación </t>
+  </si>
+  <si>
+    <t>Jorge Fernandez</t>
+  </si>
+  <si>
+    <t>12-12-2025</t>
+  </si>
+  <si>
+    <t>SOPROLE</t>
+  </si>
+  <si>
+    <t>79815300-5</t>
+  </si>
+  <si>
+    <t>MDVR 4ch sin IA</t>
+  </si>
+  <si>
+    <t>JORGE FERNANDEZ</t>
+  </si>
+  <si>
+    <t>jorge.fernandez@position.cl</t>
+  </si>
+  <si>
+    <t>EL VENTISQUERO 1250, RENCA</t>
+  </si>
+  <si>
+    <t>RENCA</t>
+  </si>
+  <si>
+    <t>Sergio Ortiz</t>
+  </si>
+  <si>
+    <t>Actividad: Instalación 
+Accesorios: GPS 
+Subcuenta de visualización: FLOTA_LUREYE 
+Marca: Sin información 
+Modelo: Sin información 
+Año: Sin informacion</t>
+  </si>
+  <si>
+    <t>Obs I+D: Favor indicar IMEI del dispositivo y nombre que se le colocó</t>
+  </si>
+  <si>
+    <t>Validación KAM: 
+1. actualizar IMEI y nombre en archivo 
+2. Incluir en carpeta respectiva 
+3. formalizar actividad.</t>
+  </si>
+  <si>
+    <t>LUREYE</t>
+  </si>
+  <si>
+    <t>77030540-3</t>
+  </si>
+  <si>
+    <t>xaviera.gatica@lureye.cl</t>
+  </si>
+  <si>
+    <t>XAVIERA GATICA</t>
+  </si>
+  <si>
+    <t>AV. LO ESPEJO 1300, MAIPU</t>
+  </si>
+  <si>
+    <t>MAIPU</t>
+  </si>
+  <si>
+    <t>29-10-2025</t>
+  </si>
+  <si>
+    <t>SANTIAGO - REVISION  GPS - INSTALACIÓN ACCESORIOS- CIAL_ALIMENTOS -HCCR38 (REVISAR GPS Y SONDA)</t>
+  </si>
+  <si>
+    <t>ACTIVIDAD: INSTALACIÓN  
+GPS  
+BOTON EMERGENCIA  
+CORTE MOTOR  
 SENSOR DE TEMPERATURA CON DOBLE SONDA 
 2 SENSOR MAGNETICO 
-RETIRO EQUIPO COMPETENCIA 
-Patente PRSV10-5 
-Tipo CAMIONETA 
-Marca KYC 
-Modelo X5 PLUS CARGO FRIO 1.8 
-Año 2021 
-Color BLANCO 
-N° Motor L01451557 
-N° Chasis LSCACN2WXME230640 
-Procedencia CHINA 
-Fabricante KYC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I+D 
-1.- DETALLAR TODO LO ENCONTRADO O REVISADO EN TERRENO 
-2.- VALIDAR POSICION DE DISPOSITIVO GPS 
-3.- VALIDACIÓN DE FUNCIONAMIENTO BOTON EMERGENCIA 
-4.- VALIDACIÓN DE FUNCIONAMIENTO CORTE MOTOR 
-5.- VALIDACIÓN DE FUNCIONAMIENTO SENSOR PUERTA 
-6.- VALIDACIÓN DE SENSOR DE TEMPERATURA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 26-12-2025 10:28
-COORDINADO CON EDUARDO PARA 05.01.25 A LAS 10:00 HRS.
-=-=
-@Carlos Ruiz 23-12-2025 16:24
-ACTIVIDAD NO RELIZADA
-=-=
-@Soledad Brito 18-12-2025 17:05
+RETIRO EQUIPO COMPETENCIA  
+Información vehicular 
+Patente  HCCR38-2 
+Tipo  CAMION 
+Marca  HINO 
+Modelo  XZU CITY 
+Año  2015 
+Color  BLANCO 
+N° Motor  N04CVC11063 
+N° Chasis  JHHACN4H3FK002344 
+Procedencia  JAPAN 
+Fabricante  HINO 
+Tipo de sello  SELLO VERDE 
+Combustible  DIESEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 18-12-2025 17:05
 COORDINADO PARA 22.10.25 A LAS 10:00 HRS.
 =-=
-@Blanca Acuña 17-12-2025 11:06
-ESTIMADOS ESTADO DE VALIDACION
+@Blanca Acuña 17-12-2025 12:30
+ESTIMADOS FAVOR APOYO CON COMENTARIOS O COORDINACIÓN
 =-=
 @Soledad Brito 10-12-2025 15:40
 COORDINADO CON ERIKSON FIGUEROA PARA 15.12.25 A LAS 10:00 HRS.
+=-=
+@Blanca Acuña 05-12-2025 11:40
+Estimados de acuerdo a lo que OP se comprometio se asistiria dia jueves
+=-=
+@Blanca Acuña 28-11-2025 17:10
+ESTIMADO CUANDO REVISEN UNIDAD FAVOR REVISAR GPS
+=-=
+@Blanca Acuña 19-11-2025 09:31
+Estimados agredecere coordinar
+=-=
+@Alejandro Medina 18-11-2025 19:04
+NUEVA INSTALACION (18-11-2025) 
+QUEDA PENDIENTE CAMBIO DE SONDA EL CUAL SERA REALIZADO MAÑANA POR EL TECNICO
+=-=
+@Soledad Brito 30-10-2025 17:44
+COORDINADO PARA EMPEZAR CON TRABAJOS DESDE 03.11.25 A LAS 10:00 HRS.
 </t>
   </si>
   <si>
-    <t>114414</t>
-  </si>
-  <si>
-    <t>PRSV10</t>
-  </si>
-  <si>
-    <t>Antena GPS, Corta Corriente Remoto</t>
-  </si>
-  <si>
-    <t>VICTOR JIMENEZ</t>
-  </si>
-  <si>
-    <t>AMERICO VESPUCIO NORTE 2341, PUDAHUEL</t>
-  </si>
-  <si>
-    <t>Instalacion</t>
+    <t>HCCR38</t>
+  </si>
+  <si>
+    <t>SANTIAGO - INSTALACIÓN GPS - ACCESORIOS- CIAL_ALIMENTOS -BSBJ91</t>
+  </si>
+  <si>
+    <t>ACTIVIDAD: INSTALACIÓN  
+GPS  
+BOTON EMERGENCIA  
+CORTE MOTOR  
+SENSOR DE TEMPERATURA CON DOBLE SONDA 
+2 SENSOR MAGNETICO 
+RETIRO EQUIPO COMPETENCIA  
+Información vehicular 
+Patente  BSBJ91-1 
+Tipo  CAMIONETA 
+Marca  KIA MOTORS 
+Modelo  FRONTIER II PLUS 2.5 
+Año  2008 
+Color  BLANCO INVIERNO 
+N° Motor  D4BH7483180 
+N° Chasis  7264620 
+Procedencia  NO DISPONIBLE 
+Fabricante  KIA MOTORS 
+Tipo de sello  SELLO VERDE 
+Combustible  DIESEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 18-12-2025 17:05
+COORDINADO PARA 22.10.25 A LAS 10:00 HRS.
+=-=
+@Blanca Acuña 17-12-2025 12:30
+ESTIMADOS FAVOR SU COMENTARIOS O COORDINACIÓN
+=-=
+@Soledad Brito 10-12-2025 15:40
+COORDINADO CON ERIKSON FIGUEROA PARA 15.12.25 A LAS 10:00 HRS.
+=-=
+@Blanca Acuña 03-12-2025 17:31
+Esta unidad si se debe instalar segun nomina entregada por nicolass
+=-=
+@Nicolas del Rio 03-12-2025 12:50
+ESTIMADOS/AS 
+JUNTO CON SALUDAR, FAVOR REVISAR ESTOS TKT. 
+SOLO QUEDAN 5 PATENTES PENDIENTES POR INSTALAR EN SANTIAGO CIAL. 
+ESTAS NO HAN SIDO DISPUESTA POR CLIENTE SEGUN LO ACORDADO PARA EL DIA LUNES 01 DIC. 
+LAS PATENTES ENTREGADAS SON LAS SIGUIENTES: 
+KLDW99 
+SW6032 
+JLKZ48 
+CVGC73 
+BSBJ91 
+CUALQUIER DUDA QUEDO ATENTO. 
+DESDE YA GRACIAS 
+SALUDOS
+</t>
+  </si>
+  <si>
+    <t>BSBJ91</t>
+  </si>
+  <si>
+    <t>17-12-2025</t>
+  </si>
+  <si>
+    <t>MACUL - SOPORTE GPS - DIBOR - VDVP13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad: REVISION DE ACCESORIO 
+Accesorio: BOTON DE EMERGENCIA 
+subcuenta visualización:  
+Año GPS: FLOTA_DIBOR 
+Marca: CHEVROLET 
+Modelo: N400 1 5 
+Año: 2025 
+Observación: CLIENTE SOLICITA CAMBIO DE UBICACION DE BOTON DE EMERGENCIA YA QUE INDICA QUE UNIDAD REGISTRA CONSTANTEMENTE EVENTOS DE ESTE ACCESORIO SOLO POR PASAR A ACCIONAR. FAVOR COODINAR ACTIVIDAD.  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 17-12-2025 14:27
+COORDINADO CON FRANCISCO BORSELLI, PARA 22.12.25 A LAS 10:30 HRS
+</t>
+  </si>
+  <si>
+    <t>COMERCIAL_DIBOR</t>
+  </si>
+  <si>
+    <t>76896060-7</t>
+  </si>
+  <si>
+    <t>109197</t>
+  </si>
+  <si>
+    <t>VDVP13</t>
+  </si>
+  <si>
+    <t>Botón Alámbrico Tablero</t>
+  </si>
+  <si>
+    <t>fborselli@dibor.cl</t>
+  </si>
+  <si>
+    <t>FRANCISCO BORSELLI</t>
+  </si>
+  <si>
+    <t>RODRIGO DE ARAYA 2821, MACUL</t>
+  </si>
+  <si>
+    <t>MACUL</t>
+  </si>
+  <si>
+    <t>alta</t>
+  </si>
+  <si>
+    <t>SANTIAGO - SOPORTE MDVR - SOPROLE - KHSJ34</t>
+  </si>
+  <si>
+    <t>Estimados por favor su apoyo con esta actividad, unidad con inconsistencia en transmision debido a que cableado de equipo se vio afectado al abrir puerta trasera del camion, donde se puede apreciar que posterior a apertura de esta, se observa que equipo deja de transmitir, ademas de quedar cableado colgando como se muestra en imagen adjunta. 
+Actividad a realizar: Revision camaras, revisar cableado por intervencion 
+Tipo CAMION 
+Marca MERCEDES BENZ 
+Modelo ATEGO 1624 
+Año 2018 
+Color BLANCO 
+N° Motor 902916C1123305 
+N° Chasis WDB970078H0100495 
+Procedencia GERMANY 
+Fabricante MERCEDES-BENZ &amp; MAYBACH 
+Tipo de sello SELLO VERDE 
+Combustible DIESEL</t>
+  </si>
+  <si>
+    <t>I+D 
+1.- VALIDAR ACTIVIDAD 
+2.- VALIDAR POSICION Y EVENTOS DE MDVR 
+3.- VALIDAR CORRECTO FUNCIONAMIENTO DE MDVR Y CAMARAS 
+4.- ADJUNTAR IMAGENES DE VEHICULO, MDVR Y CAMARAS 
+5.- INDICAR LO QUE SE REALIZO PARA DEJAR OPERATIVO EQUIPO 
+6.- SUB CUENTA VISUALIZACION: FLOTA_SOPROLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 17-12-2025 12:03
+RECOORDINADO PARA 17. Y 18 DEL 12.25 A LAS 15:00 
+=-=
+@Joaquin Lopez 17-12-2025 08:52
+TECNICO ESPERO EL VEHICULO PERO NO LLEGO
+=-=
+@Soledad Brito 12-12-2025 12:35
+COORDINADO PARA 16.12.25 A LAS 15:00 HRS.
+</t>
+  </si>
+  <si>
+    <t>97801</t>
+  </si>
+  <si>
+    <t>KHSJ34</t>
+  </si>
+  <si>
+    <t>09-12-2025</t>
+  </si>
+  <si>
+    <t>15-12-2025</t>
+  </si>
+  <si>
+    <t>MAIPU- INSTALACIÓN - LUREYE - GENERADOR_SANTIAGO_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 15-12-2025 11:51
+COORDINADO DESDE 16.12.25
+=-=
+@Soledad Brito 10-12-2025 11:29
+COORDINADO DESDE 10-12.25 A LAS 10:00 HRS. TECNICO FABIAN DIAZ
+</t>
+  </si>
+  <si>
+    <t>GENERADOR_SANTIAGO_19</t>
+  </si>
+  <si>
+    <t>MAIPU- INSTALACIÓN - LUREYE - GENERADOR_SANTIAGO_18</t>
+  </si>
+  <si>
+    <t>GENERADOR_SANTIAGO_18</t>
   </si>
 </sst>
 </file>
@@ -1365,11 +1464,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A85CC9B-2657-4742-8687-9E1AA5B38A74}">
-  <dimension ref="A1:BG5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C151FAE8-D70A-460F-8954-F98809C848D1}">
+  <dimension ref="A1:BG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1562,19 +1661,19 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>42944</v>
+        <v>41335</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
         <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
         <v>63</v>
@@ -1589,97 +1688,97 @@
         <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="L2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" t="s">
         <v>67</v>
       </c>
-      <c r="M2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" t="s">
-        <v>61</v>
-      </c>
-      <c r="O2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>109</v>
+      </c>
+      <c r="U2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" t="s">
+        <v>110</v>
+      </c>
+      <c r="W2" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y2">
+        <v>8</v>
+      </c>
+      <c r="Z2">
+        <v>8</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" t="s">
         <v>68</v>
-      </c>
-      <c r="T2" t="s">
-        <v>75</v>
-      </c>
-      <c r="U2" t="s">
-        <v>61</v>
-      </c>
-      <c r="V2" t="s">
-        <v>76</v>
-      </c>
-      <c r="W2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>69</v>
       </c>
       <c r="AE2">
         <v>24</v>
       </c>
       <c r="AF2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AG2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AH2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AI2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="AJ2" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="AK2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL2" t="s">
         <v>72</v>
       </c>
-      <c r="AL2" t="s">
-        <v>81</v>
-      </c>
       <c r="AM2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="AN2" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="AO2" t="s">
         <v>61</v>
@@ -1694,16 +1793,16 @@
         <v>61</v>
       </c>
       <c r="AS2" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="AT2">
-        <v>0</v>
+        <v>978079214</v>
       </c>
       <c r="AU2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AV2" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="AW2" t="s">
         <v>61</v>
@@ -1715,19 +1814,19 @@
         <v>61</v>
       </c>
       <c r="AZ2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BA2" t="s">
         <v>83</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2">
+        <v>978079214</v>
+      </c>
+      <c r="BC2" t="s">
         <v>84</v>
       </c>
-      <c r="BB2">
-        <v>56996301286</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>85</v>
-      </c>
       <c r="BD2" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="BE2" t="s">
         <v>61</v>
@@ -1741,19 +1840,19 @@
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>42965</v>
+        <v>41321</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
         <v>63</v>
@@ -1762,103 +1861,103 @@
         <v>64</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="K3" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="L3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" t="s">
+        <v>61</v>
+      </c>
+      <c r="S3" t="s">
         <v>67</v>
       </c>
-      <c r="M3" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" t="s">
-        <v>61</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
+        <v>113</v>
+      </c>
+      <c r="U3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" t="s">
+        <v>114</v>
+      </c>
+      <c r="W3" t="s">
+        <v>87</v>
+      </c>
+      <c r="X3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD3" t="s">
         <v>68</v>
-      </c>
-      <c r="T3" t="s">
-        <v>99</v>
-      </c>
-      <c r="U3" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" t="s">
-        <v>100</v>
-      </c>
-      <c r="W3" t="s">
-        <v>61</v>
-      </c>
-      <c r="X3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y3">
-        <v>12</v>
-      </c>
-      <c r="Z3">
-        <v>4</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>69</v>
       </c>
       <c r="AE3">
         <v>24</v>
       </c>
       <c r="AF3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AG3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="AH3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AI3" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="AJ3" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="AK3" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="AL3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="AM3" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="AN3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AO3" t="s">
         <v>61</v>
@@ -1873,16 +1972,16 @@
         <v>61</v>
       </c>
       <c r="AS3" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="AT3">
-        <v>0</v>
+        <v>978079214</v>
       </c>
       <c r="AU3" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="AV3" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="AW3" t="s">
         <v>61</v>
@@ -1894,25 +1993,25 @@
         <v>61</v>
       </c>
       <c r="AZ3" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="BA3" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="BB3">
-        <v>939592260</v>
+        <v>978079214</v>
       </c>
       <c r="BC3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="BD3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="BE3" t="s">
         <v>61</v>
       </c>
       <c r="BF3" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="BG3" t="s">
         <v>61</v>
@@ -1920,19 +2019,19 @@
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>43007</v>
+        <v>42884</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
         <v>63</v>
@@ -1947,49 +2046,49 @@
         <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K4" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="L4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" t="s">
         <v>67</v>
       </c>
-      <c r="M4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" t="s">
-        <v>61</v>
-      </c>
-      <c r="O4" t="s">
-        <v>61</v>
-      </c>
-      <c r="P4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>61</v>
-      </c>
-      <c r="R4" t="s">
-        <v>61</v>
-      </c>
-      <c r="S4" t="s">
-        <v>68</v>
-      </c>
       <c r="T4" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="U4" t="s">
         <v>61</v>
       </c>
       <c r="V4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="W4" t="s">
         <v>61</v>
       </c>
       <c r="X4" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -1998,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="AA4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="AB4" t="s">
         <v>61</v>
@@ -2007,37 +2106,37 @@
         <v>61</v>
       </c>
       <c r="AD4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE4">
         <v>24</v>
       </c>
       <c r="AF4" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="AG4" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="AH4" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="AI4" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="AJ4" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="AK4" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="AL4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="AM4" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="AN4" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="AO4" t="s">
         <v>61</v>
@@ -2058,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="AU4" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="AV4" t="s">
         <v>61</v>
@@ -2073,19 +2172,19 @@
         <v>61</v>
       </c>
       <c r="AZ4" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="BA4" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="BB4">
-        <v>953964686</v>
+        <v>987388706</v>
       </c>
       <c r="BC4" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="BD4" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="BE4" t="s">
         <v>61</v>
@@ -2099,19 +2198,19 @@
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>42730</v>
+        <v>42794</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="F5" t="s">
         <v>63</v>
@@ -2126,162 +2225,515 @@
         <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="K5" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="L5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" t="s">
+        <v>61</v>
+      </c>
+      <c r="O5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" t="s">
         <v>67</v>
       </c>
-      <c r="M5" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" t="s">
-        <v>61</v>
-      </c>
-      <c r="O5" t="s">
-        <v>61</v>
-      </c>
-      <c r="P5" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" t="s">
-        <v>61</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
+        <v>131</v>
+      </c>
+      <c r="U5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V5" t="s">
+        <v>132</v>
+      </c>
+      <c r="W5" t="s">
+        <v>61</v>
+      </c>
+      <c r="X5" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y5">
+        <v>4</v>
+      </c>
+      <c r="Z5">
+        <v>3</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD5" t="s">
         <v>68</v>
-      </c>
-      <c r="T5" t="s">
-        <v>121</v>
-      </c>
-      <c r="U5" t="s">
-        <v>61</v>
-      </c>
-      <c r="V5" t="s">
-        <v>122</v>
-      </c>
-      <c r="W5" t="s">
-        <v>61</v>
-      </c>
-      <c r="X5" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y5">
-        <v>1</v>
-      </c>
-      <c r="Z5">
-        <v>5</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>124</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>69</v>
       </c>
       <c r="AE5">
         <v>24</v>
       </c>
       <c r="AF5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG5" t="s">
         <v>92</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM5" t="s">
         <v>93</v>
       </c>
-      <c r="AH5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>125</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK5" t="s">
+      <c r="AN5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS5" t="s">
         <v>94</v>
       </c>
-      <c r="AL5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>127</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>61</v>
-      </c>
       <c r="AT5">
+        <v>952072432</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>94</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>96</v>
+      </c>
+      <c r="BB5">
+        <v>952072432</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>97</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>42679</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" t="s">
+        <v>137</v>
+      </c>
+      <c r="L6" t="s">
+        <v>138</v>
+      </c>
+      <c r="M6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R6" t="s">
+        <v>61</v>
+      </c>
+      <c r="S6" t="s">
+        <v>67</v>
+      </c>
+      <c r="T6" t="s">
+        <v>139</v>
+      </c>
+      <c r="U6" t="s">
+        <v>61</v>
+      </c>
+      <c r="V6" t="s">
+        <v>99</v>
+      </c>
+      <c r="W6" t="s">
+        <v>100</v>
+      </c>
+      <c r="X6" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y6">
         <v>0</v>
       </c>
-      <c r="AU5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>128</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>129</v>
-      </c>
-      <c r="BB5">
-        <v>978079214</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>119</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>86</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>61</v>
-      </c>
-      <c r="BG5" t="s">
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE6">
+        <v>24</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>105</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>106</v>
+      </c>
+      <c r="BB6">
+        <v>978263964</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>61</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>61</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>42678</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" t="s">
+        <v>137</v>
+      </c>
+      <c r="L7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" t="s">
+        <v>61</v>
+      </c>
+      <c r="S7" t="s">
+        <v>67</v>
+      </c>
+      <c r="T7" t="s">
+        <v>142</v>
+      </c>
+      <c r="U7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V7" t="s">
+        <v>99</v>
+      </c>
+      <c r="W7" t="s">
+        <v>100</v>
+      </c>
+      <c r="X7" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE7">
+        <v>24</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>105</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BB7">
+        <v>978263964</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>61</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>61</v>
+      </c>
+      <c r="BG7" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BG17" xr:uid="{5A85CC9B-2657-4742-8687-9E1AA5B38A74}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BG17">
-      <sortCondition descending="1" ref="J1:J17"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement Points System Backend and Mobile App Integration
</commit_message>
<xml_diff>
--- a/backend/Coordinados (11).xlsx
+++ b/backend/Coordinados (11).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA37CA90-A6B0-485F-BA68-006FFD55D342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBDE56E9-DFAE-4412-A1DD-05E833C9F508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{F9CA0F41-2E70-4754-8728-A810F4F5D8DC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{2EED89DB-939F-41DF-829A-0C8715EB1109}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinados" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="90">
   <si>
     <t>ID</t>
   </si>
@@ -202,409 +202,115 @@
     <t>Coordinados</t>
   </si>
   <si>
-    <t>José Cabrera</t>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>menor</t>
+  </si>
+  <si>
+    <t>no se ha intentado</t>
+  </si>
+  <si>
+    <t>nueva</t>
+  </si>
+  <si>
+    <t>abierta</t>
+  </si>
+  <si>
+    <t>Instalación</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>inmediata</t>
-  </si>
-  <si>
-    <t>menor</t>
-  </si>
-  <si>
-    <t>no se ha intentado</t>
-  </si>
-  <si>
-    <t>nueva</t>
-  </si>
-  <si>
-    <t>abierta</t>
-  </si>
-  <si>
     <t>público</t>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
-    <t>Arriendo</t>
-  </si>
-  <si>
-    <t>Soporte</t>
-  </si>
-  <si>
-    <t>18-12-2025</t>
+    <t>Camión</t>
   </si>
   <si>
     <t>GV310LAU</t>
   </si>
   <si>
-    <t>Región Metropolitana de Santiago.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Soporte</t>
-  </si>
-  <si>
-    <t>Blanca Acuña</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>Antena GPS</t>
-  </si>
-  <si>
-    <t>Vehículo</t>
-  </si>
-  <si>
-    <t>CIAL_ALIMENTOS</t>
-  </si>
-  <si>
-    <t>80186300-0</t>
-  </si>
-  <si>
-    <t>Camión</t>
-  </si>
-  <si>
-    <t>Instalación</t>
-  </si>
-  <si>
-    <t>AMERICO VESPUCIO 2341 PUDAHUEL</t>
-  </si>
-  <si>
-    <t>PUDAHUEL</t>
-  </si>
-  <si>
-    <t>VICTOR JIMENEZ</t>
-  </si>
-  <si>
-    <t>nicolas.zuniga@cial.cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDACIÓN I+D  
-1.- VALIDAR POSICION DE DISPOSITIVO GPS  
-2.- VALIDACIÓN DE FUNCIONAMIENTO BOTON EMERGENCIA  
-3.- VALIDACIÓN DE FUNCIONAMIENTO CORTE MOTOR  
-4.- VALIDACIÓN DE FUNCIONAMIENTO SENSOR PUERTA  
-5.- VALIDACIÓN DE SENSOR DE TEMPERATURA (AMBAS SONDAS DEBEN ESTAR FUNCIONALES) 
-6.- FOTOGRAFIA DE GPS COMPETENCIA (NUMERO DE SERIE)  
-7.- FOTOGRAFÍA FISICA DE LA UBICACIÓN DEL GPS (DONDE QUEDA INSTALADO) (OBLIGATORIO) 
-8.- FOTOGRAFÍA DE PATENTE INTERVENIDA  
-9.- OT FIRMADA  
-10.- DAR VISUALIZACIÓN A SUBCUENTA FLOTA_CIALALIMENTOS 
-ZONA Y ALARMA  
-1.- VELOCIDAD 95 KM POR 1 MINUTO  
-2.- CARGA DE ZONAS POR ACCESORIOS IMPLEMENTADOS  
-3.- CARGAR ALARMA DE TEMPERATURA PEGADA  
-4.- SIN COBERTURA GPS  
+    <t>Región de Antofagasta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalación </t>
+  </si>
+  <si>
+    <t>Yessica Santibañez</t>
+  </si>
+  <si>
+    <t>PENDIENTE</t>
+  </si>
+  <si>
+    <t>CALLE N°8 SITIO N°6 MZA K SECTOR PUERTO SECO. CALAMA</t>
+  </si>
+  <si>
+    <t>10-12-2025</t>
+  </si>
+  <si>
+    <t>CALAMA - INSTALACION MVDR4 IA + DMS + ADAS + CAMARA V4- AGRETRANS - X</t>
+  </si>
+  <si>
+    <t>AGRETRANS LOA</t>
+  </si>
+  <si>
+    <t>75584300-8</t>
+  </si>
+  <si>
+    <t>MDVR 4ch con IA, V4, DMS, ADAS</t>
+  </si>
+  <si>
+    <t>CARLOS ORTEGA</t>
+  </si>
+  <si>
+    <t>administrador.dch@agretrans.cl</t>
+  </si>
+  <si>
+    <t>26-11-2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVIDAD: MVDR4 + DMS + ADAS 
+Patente  
+Tipo TRACTOCAMION 
+Marca  
+Modelo  
+Año  
+Color  
+N° Motor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   I+D 
+Favor validar correcto funcionamiento 
+1.- Validación transmisión GPS y latencia cada 30 seg 
+2.- Cargar zona y alarmas accesorios 
+3.- Validación accesorios en Plataforma 
+4.- funcionamiento inteligencia artificial mas calibración 
+5.- validar inteligencia artificial modulo evidencia, Ojos cerrados, uso de telefono (VSS) 
+6.- MVDR debe entregar posicionamiento (VALIDAR SATELITES) 
+7.- validar transmisión en línea de cámaras 
+8.- fotografía de Disco duro 
+9.- Respaldo OT 
+10.-Conectar a intermitentes 
+11.- SIMCARD CLARO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 10-12-2025 17:10
+COORDINADO DESDE 11.12.25 TECNICO: ORLANDO LUGO
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Instalación </t>
-  </si>
-  <si>
-    <t>Jorge Fernandez</t>
-  </si>
-  <si>
-    <t>12-12-2025</t>
-  </si>
-  <si>
-    <t>SOPROLE</t>
-  </si>
-  <si>
-    <t>79815300-5</t>
-  </si>
-  <si>
-    <t>MDVR 4ch sin IA</t>
-  </si>
-  <si>
-    <t>JORGE FERNANDEZ</t>
-  </si>
-  <si>
-    <t>jorge.fernandez@position.cl</t>
-  </si>
-  <si>
-    <t>EL VENTISQUERO 1250, RENCA</t>
-  </si>
-  <si>
-    <t>RENCA</t>
-  </si>
-  <si>
-    <t>Sergio Ortiz</t>
-  </si>
-  <si>
-    <t>Actividad: Instalación 
-Accesorios: GPS 
-Subcuenta de visualización: FLOTA_LUREYE 
-Marca: Sin información 
-Modelo: Sin información 
-Año: Sin informacion</t>
-  </si>
-  <si>
-    <t>Obs I+D: Favor indicar IMEI del dispositivo y nombre que se le colocó</t>
-  </si>
-  <si>
-    <t>Validación KAM: 
-1. actualizar IMEI y nombre en archivo 
-2. Incluir en carpeta respectiva 
-3. formalizar actividad.</t>
-  </si>
-  <si>
-    <t>LUREYE</t>
-  </si>
-  <si>
-    <t>77030540-3</t>
-  </si>
-  <si>
-    <t>xaviera.gatica@lureye.cl</t>
-  </si>
-  <si>
-    <t>XAVIERA GATICA</t>
-  </si>
-  <si>
-    <t>AV. LO ESPEJO 1300, MAIPU</t>
-  </si>
-  <si>
-    <t>MAIPU</t>
-  </si>
-  <si>
-    <t>29-10-2025</t>
-  </si>
-  <si>
-    <t>SANTIAGO - REVISION  GPS - INSTALACIÓN ACCESORIOS- CIAL_ALIMENTOS -HCCR38 (REVISAR GPS Y SONDA)</t>
-  </si>
-  <si>
-    <t>ACTIVIDAD: INSTALACIÓN  
-GPS  
-BOTON EMERGENCIA  
-CORTE MOTOR  
-SENSOR DE TEMPERATURA CON DOBLE SONDA 
-2 SENSOR MAGNETICO 
-RETIRO EQUIPO COMPETENCIA  
-Información vehicular 
-Patente  HCCR38-2 
-Tipo  CAMION 
-Marca  HINO 
-Modelo  XZU CITY 
-Año  2015 
-Color  BLANCO 
-N° Motor  N04CVC11063 
-N° Chasis  JHHACN4H3FK002344 
-Procedencia  JAPAN 
-Fabricante  HINO 
-Tipo de sello  SELLO VERDE 
-Combustible  DIESEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 18-12-2025 17:05
-COORDINADO PARA 22.10.25 A LAS 10:00 HRS.
-=-=
-@Blanca Acuña 17-12-2025 12:30
-ESTIMADOS FAVOR APOYO CON COMENTARIOS O COORDINACIÓN
-=-=
-@Soledad Brito 10-12-2025 15:40
-COORDINADO CON ERIKSON FIGUEROA PARA 15.12.25 A LAS 10:00 HRS.
-=-=
-@Blanca Acuña 05-12-2025 11:40
-Estimados de acuerdo a lo que OP se comprometio se asistiria dia jueves
-=-=
-@Blanca Acuña 28-11-2025 17:10
-ESTIMADO CUANDO REVISEN UNIDAD FAVOR REVISAR GPS
-=-=
-@Blanca Acuña 19-11-2025 09:31
-Estimados agredecere coordinar
-=-=
-@Alejandro Medina 18-11-2025 19:04
-NUEVA INSTALACION (18-11-2025) 
-QUEDA PENDIENTE CAMBIO DE SONDA EL CUAL SERA REALIZADO MAÑANA POR EL TECNICO
-=-=
-@Soledad Brito 30-10-2025 17:44
-COORDINADO PARA EMPEZAR CON TRABAJOS DESDE 03.11.25 A LAS 10:00 HRS.
-</t>
-  </si>
-  <si>
-    <t>HCCR38</t>
-  </si>
-  <si>
-    <t>SANTIAGO - INSTALACIÓN GPS - ACCESORIOS- CIAL_ALIMENTOS -BSBJ91</t>
-  </si>
-  <si>
-    <t>ACTIVIDAD: INSTALACIÓN  
-GPS  
-BOTON EMERGENCIA  
-CORTE MOTOR  
-SENSOR DE TEMPERATURA CON DOBLE SONDA 
-2 SENSOR MAGNETICO 
-RETIRO EQUIPO COMPETENCIA  
-Información vehicular 
-Patente  BSBJ91-1 
-Tipo  CAMIONETA 
-Marca  KIA MOTORS 
-Modelo  FRONTIER II PLUS 2.5 
-Año  2008 
-Color  BLANCO INVIERNO 
-N° Motor  D4BH7483180 
-N° Chasis  7264620 
-Procedencia  NO DISPONIBLE 
-Fabricante  KIA MOTORS 
-Tipo de sello  SELLO VERDE 
-Combustible  DIESEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 18-12-2025 17:05
-COORDINADO PARA 22.10.25 A LAS 10:00 HRS.
-=-=
-@Blanca Acuña 17-12-2025 12:30
-ESTIMADOS FAVOR SU COMENTARIOS O COORDINACIÓN
-=-=
-@Soledad Brito 10-12-2025 15:40
-COORDINADO CON ERIKSON FIGUEROA PARA 15.12.25 A LAS 10:00 HRS.
-=-=
-@Blanca Acuña 03-12-2025 17:31
-Esta unidad si se debe instalar segun nomina entregada por nicolass
-=-=
-@Nicolas del Rio 03-12-2025 12:50
-ESTIMADOS/AS 
-JUNTO CON SALUDAR, FAVOR REVISAR ESTOS TKT. 
-SOLO QUEDAN 5 PATENTES PENDIENTES POR INSTALAR EN SANTIAGO CIAL. 
-ESTAS NO HAN SIDO DISPUESTA POR CLIENTE SEGUN LO ACORDADO PARA EL DIA LUNES 01 DIC. 
-LAS PATENTES ENTREGADAS SON LAS SIGUIENTES: 
-KLDW99 
-SW6032 
-JLKZ48 
-CVGC73 
-BSBJ91 
-CUALQUIER DUDA QUEDO ATENTO. 
-DESDE YA GRACIAS 
-SALUDOS
-</t>
-  </si>
-  <si>
-    <t>BSBJ91</t>
-  </si>
-  <si>
-    <t>17-12-2025</t>
-  </si>
-  <si>
-    <t>MACUL - SOPORTE GPS - DIBOR - VDVP13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad: REVISION DE ACCESORIO 
-Accesorio: BOTON DE EMERGENCIA 
-subcuenta visualización:  
-Año GPS: FLOTA_DIBOR 
-Marca: CHEVROLET 
-Modelo: N400 1 5 
-Año: 2025 
-Observación: CLIENTE SOLICITA CAMBIO DE UBICACION DE BOTON DE EMERGENCIA YA QUE INDICA QUE UNIDAD REGISTRA CONSTANTEMENTE EVENTOS DE ESTE ACCESORIO SOLO POR PASAR A ACCIONAR. FAVOR COODINAR ACTIVIDAD.  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 17-12-2025 14:27
-COORDINADO CON FRANCISCO BORSELLI, PARA 22.12.25 A LAS 10:30 HRS
-</t>
-  </si>
-  <si>
-    <t>COMERCIAL_DIBOR</t>
-  </si>
-  <si>
-    <t>76896060-7</t>
-  </si>
-  <si>
-    <t>109197</t>
-  </si>
-  <si>
-    <t>VDVP13</t>
-  </si>
-  <si>
-    <t>Botón Alámbrico Tablero</t>
-  </si>
-  <si>
-    <t>fborselli@dibor.cl</t>
-  </si>
-  <si>
-    <t>FRANCISCO BORSELLI</t>
-  </si>
-  <si>
-    <t>RODRIGO DE ARAYA 2821, MACUL</t>
-  </si>
-  <si>
-    <t>MACUL</t>
-  </si>
-  <si>
-    <t>alta</t>
-  </si>
-  <si>
-    <t>SANTIAGO - SOPORTE MDVR - SOPROLE - KHSJ34</t>
-  </si>
-  <si>
-    <t>Estimados por favor su apoyo con esta actividad, unidad con inconsistencia en transmision debido a que cableado de equipo se vio afectado al abrir puerta trasera del camion, donde se puede apreciar que posterior a apertura de esta, se observa que equipo deja de transmitir, ademas de quedar cableado colgando como se muestra en imagen adjunta. 
-Actividad a realizar: Revision camaras, revisar cableado por intervencion 
-Tipo CAMION 
-Marca MERCEDES BENZ 
-Modelo ATEGO 1624 
-Año 2018 
-Color BLANCO 
-N° Motor 902916C1123305 
-N° Chasis WDB970078H0100495 
-Procedencia GERMANY 
-Fabricante MERCEDES-BENZ &amp; MAYBACH 
-Tipo de sello SELLO VERDE 
-Combustible DIESEL</t>
-  </si>
-  <si>
-    <t>I+D 
-1.- VALIDAR ACTIVIDAD 
-2.- VALIDAR POSICION Y EVENTOS DE MDVR 
-3.- VALIDAR CORRECTO FUNCIONAMIENTO DE MDVR Y CAMARAS 
-4.- ADJUNTAR IMAGENES DE VEHICULO, MDVR Y CAMARAS 
-5.- INDICAR LO QUE SE REALIZO PARA DEJAR OPERATIVO EQUIPO 
-6.- SUB CUENTA VISUALIZACION: FLOTA_SOPROLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 17-12-2025 12:03
-RECOORDINADO PARA 17. Y 18 DEL 12.25 A LAS 15:00 
-=-=
-@Joaquin Lopez 17-12-2025 08:52
-TECNICO ESPERO EL VEHICULO PERO NO LLEGO
-=-=
-@Soledad Brito 12-12-2025 12:35
-COORDINADO PARA 16.12.25 A LAS 15:00 HRS.
-</t>
-  </si>
-  <si>
-    <t>97801</t>
-  </si>
-  <si>
-    <t>KHSJ34</t>
-  </si>
-  <si>
-    <t>09-12-2025</t>
-  </si>
-  <si>
-    <t>15-12-2025</t>
-  </si>
-  <si>
-    <t>MAIPU- INSTALACIÓN - LUREYE - GENERADOR_SANTIAGO_19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 15-12-2025 11:51
-COORDINADO DESDE 16.12.25
-=-=
-@Soledad Brito 10-12-2025 11:29
-COORDINADO DESDE 10-12.25 A LAS 10:00 HRS. TECNICO FABIAN DIAZ
-</t>
-  </si>
-  <si>
-    <t>GENERADOR_SANTIAGO_19</t>
-  </si>
-  <si>
-    <t>MAIPU- INSTALACIÓN - LUREYE - GENERADOR_SANTIAGO_18</t>
-  </si>
-  <si>
-    <t>GENERADOR_SANTIAGO_18</t>
+    <t>CALAMA - INSTALACION MVDR4 IA + DMS + ADAS + CAMARA V4 - AGRETRANS - X</t>
+  </si>
+  <si>
+    <t>MDVR 4ch con IA, DMS, ADAS</t>
+  </si>
+  <si>
+    <t>CALAMA - INSTALACION MVDR4 IA + DMS + ADAS+ CAMARA V4 - AGRETRANS - X</t>
   </si>
 </sst>
 </file>
@@ -1464,11 +1170,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C151FAE8-D70A-460F-8954-F98809C848D1}">
-  <dimension ref="A1:BG7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B82D388-9366-481A-8E12-BC3B17FE4142}">
+  <dimension ref="A1:BG5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1661,91 +1367,91 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>41335</v>
+        <v>42329</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
         <v>61</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" t="s">
         <v>76</v>
       </c>
-      <c r="F2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L2" t="s">
-        <v>71</v>
-      </c>
       <c r="M2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="O2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S2" t="s">
         <v>67</v>
       </c>
       <c r="T2" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="U2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="V2" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="W2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="X2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Y2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="AB2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AC2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AD2" t="s">
         <v>68</v>
@@ -1754,177 +1460,177 @@
         <v>24</v>
       </c>
       <c r="AF2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG2" t="s">
         <v>79</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM2" t="s">
         <v>80</v>
       </c>
-      <c r="AH2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL2" t="s">
+      <c r="AN2" t="s">
         <v>72</v>
       </c>
-      <c r="AM2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>88</v>
-      </c>
       <c r="AO2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AP2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AQ2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AR2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AS2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AT2">
-        <v>978079214</v>
+        <v>56993093036</v>
       </c>
       <c r="AU2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="AV2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="AW2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AX2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AY2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AZ2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="BA2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="BB2">
-        <v>978079214</v>
+        <v>56993093036</v>
       </c>
       <c r="BC2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="BD2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="BE2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="BF2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="BG2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>41321</v>
+        <v>42328</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
         <v>61</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" t="s">
         <v>76</v>
       </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L3" t="s">
-        <v>71</v>
-      </c>
       <c r="M3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="O3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="P3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="R3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S3" t="s">
         <v>67</v>
       </c>
       <c r="T3" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="U3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="V3" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="W3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="X3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AA3" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="AB3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AC3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AD3" t="s">
         <v>68</v>
@@ -1933,162 +1639,162 @@
         <v>24</v>
       </c>
       <c r="AF3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG3" t="s">
         <v>79</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM3" t="s">
         <v>80</v>
       </c>
-      <c r="AH3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL3" t="s">
+      <c r="AN3" t="s">
         <v>72</v>
       </c>
-      <c r="AM3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>88</v>
-      </c>
       <c r="AO3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AP3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AQ3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AR3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AS3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AT3">
-        <v>978079214</v>
+        <v>56993093036</v>
       </c>
       <c r="AU3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="AV3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="AW3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AX3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AY3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AZ3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="BA3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="BB3">
-        <v>978079214</v>
+        <v>56993093036</v>
       </c>
       <c r="BC3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="BD3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="BE3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="BF3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="BG3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>42884</v>
+        <v>42327</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>63</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>64</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>65</v>
       </c>
-      <c r="I4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J4" t="s">
-        <v>70</v>
-      </c>
       <c r="K4" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="L4" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="O4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="R4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S4" t="s">
         <v>67</v>
       </c>
       <c r="T4" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="U4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="V4" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="W4" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="X4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -2097,13 +1803,13 @@
         <v>1</v>
       </c>
       <c r="AA4" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="AB4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AC4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AD4" t="s">
         <v>68</v>
@@ -2112,177 +1818,177 @@
         <v>24</v>
       </c>
       <c r="AF4" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="AG4" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="AH4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK4" t="s">
         <v>69</v>
       </c>
-      <c r="AI4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS4" t="s">
         <v>81</v>
       </c>
-      <c r="AL4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>61</v>
-      </c>
       <c r="AT4">
-        <v>0</v>
+        <v>56993093036</v>
       </c>
       <c r="AU4" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="AV4" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="AW4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AX4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AY4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AZ4" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="BA4" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="BB4">
-        <v>987388706</v>
+        <v>56993093036</v>
       </c>
       <c r="BC4" t="s">
-        <v>129</v>
+        <v>66</v>
       </c>
       <c r="BD4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="BE4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="BF4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="BG4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>42794</v>
+        <v>42326</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s">
         <v>61</v>
       </c>
-      <c r="E5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" t="s">
         <v>63</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>64</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>65</v>
       </c>
-      <c r="I5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" t="s">
-        <v>70</v>
-      </c>
       <c r="K5" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="L5" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="M5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="O5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="P5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="R5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="S5" t="s">
         <v>67</v>
       </c>
       <c r="T5" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="U5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="V5" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="W5" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="X5" t="s">
-        <v>133</v>
+        <v>66</v>
       </c>
       <c r="Y5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AA5" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="AB5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AC5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AD5" t="s">
         <v>68</v>
@@ -2291,446 +1997,88 @@
         <v>24</v>
       </c>
       <c r="AF5" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="AG5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="AH5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK5" t="s">
         <v>69</v>
       </c>
-      <c r="AI5" t="s">
-        <v>135</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>136</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>78</v>
-      </c>
       <c r="AL5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN5" t="s">
         <v>72</v>
       </c>
-      <c r="AM5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>61</v>
-      </c>
       <c r="AO5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AP5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AQ5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AR5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AS5" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="AT5">
-        <v>952072432</v>
+        <v>56993093036</v>
       </c>
       <c r="AU5" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="AV5" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="AW5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AX5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AY5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AZ5" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="BA5" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="BB5">
-        <v>952072432</v>
+        <v>56993093036</v>
       </c>
       <c r="BC5" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="BD5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="BE5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="BF5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="BG5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>42679</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" t="s">
-        <v>82</v>
-      </c>
-      <c r="K6" t="s">
-        <v>137</v>
-      </c>
-      <c r="L6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M6" t="s">
-        <v>61</v>
-      </c>
-      <c r="N6" t="s">
-        <v>61</v>
-      </c>
-      <c r="O6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P6" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>61</v>
-      </c>
-      <c r="R6" t="s">
-        <v>61</v>
-      </c>
-      <c r="S6" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" t="s">
-        <v>139</v>
-      </c>
-      <c r="U6" t="s">
-        <v>61</v>
-      </c>
-      <c r="V6" t="s">
-        <v>99</v>
-      </c>
-      <c r="W6" t="s">
-        <v>100</v>
-      </c>
-      <c r="X6" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>2</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE6">
-        <v>24</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AT6">
-        <v>0</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>105</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>106</v>
-      </c>
-      <c r="BB6">
-        <v>978263964</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>107</v>
-      </c>
-      <c r="BD6" t="s">
-        <v>73</v>
-      </c>
-      <c r="BE6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF6" t="s">
-        <v>61</v>
-      </c>
-      <c r="BG6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>42678</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7" t="s">
-        <v>82</v>
-      </c>
-      <c r="K7" t="s">
-        <v>137</v>
-      </c>
-      <c r="L7" t="s">
-        <v>138</v>
-      </c>
-      <c r="M7" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" t="s">
-        <v>61</v>
-      </c>
-      <c r="O7" t="s">
-        <v>61</v>
-      </c>
-      <c r="P7" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>61</v>
-      </c>
-      <c r="R7" t="s">
-        <v>61</v>
-      </c>
-      <c r="S7" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" t="s">
-        <v>142</v>
-      </c>
-      <c r="U7" t="s">
-        <v>61</v>
-      </c>
-      <c r="V7" t="s">
-        <v>99</v>
-      </c>
-      <c r="W7" t="s">
-        <v>100</v>
-      </c>
-      <c r="X7" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>2</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE7">
-        <v>24</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>102</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>143</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>77</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AT7">
-        <v>0</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>107</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>105</v>
-      </c>
-      <c r="BA7" t="s">
-        <v>106</v>
-      </c>
-      <c r="BB7">
-        <v>978263964</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>107</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>73</v>
-      </c>
-      <c r="BE7" t="s">
-        <v>61</v>
-      </c>
-      <c r="BF7" t="s">
-        <v>61</v>
-      </c>
-      <c r="BG7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automate Scores Update on Signature
</commit_message>
<xml_diff>
--- a/backend/Coordinados (11).xlsx
+++ b/backend/Coordinados (11).xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBDE56E9-DFAE-4412-A1DD-05E833C9F508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3CDDCE4-2EC1-4337-BCDA-FEFEEA9A286C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{2EED89DB-939F-41DF-829A-0C8715EB1109}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{CFC39CBD-85D8-496E-ADDF-C53937D27CDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinados" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coordinados!$A$1:$BG$7</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="122">
   <si>
     <t>ID</t>
   </si>
@@ -202,6 +205,9 @@
     <t>Coordinados</t>
   </si>
   <si>
+    <t>Sergio Ortiz</t>
+  </si>
+  <si>
     <t>normal</t>
   </si>
   <si>
@@ -235,12 +241,24 @@
     <t>GV310LAU</t>
   </si>
   <si>
+    <t>Antena GPS</t>
+  </si>
+  <si>
     <t>Región de Antofagasta.</t>
   </si>
   <si>
+    <t>TEMUCO</t>
+  </si>
+  <si>
+    <t>Región de La Araucanía.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Instalación </t>
   </si>
   <si>
+    <t>Soporte</t>
+  </si>
+  <si>
     <t>Yessica Santibañez</t>
   </si>
   <si>
@@ -250,10 +268,129 @@
     <t>CALLE N°8 SITIO N°6 MZA K SECTOR PUERTO SECO. CALAMA</t>
   </si>
   <si>
+    <t>Región Metropolitana de Santiago.</t>
+  </si>
+  <si>
+    <t>18-12-2025</t>
+  </si>
+  <si>
     <t>10-12-2025</t>
   </si>
   <si>
-    <t>CALAMA - INSTALACION MVDR4 IA + DMS + ADAS + CAMARA V4- AGRETRANS - X</t>
+    <t>Constanza Barrios</t>
+  </si>
+  <si>
+    <t>22-12-2025</t>
+  </si>
+  <si>
+    <t>TEMUCO - CAMBIO DE GPS - BRINKS -SWZK97-MOV23032</t>
+  </si>
+  <si>
+    <t>ACTIVIDAD: CAMBIO DE GPS  
+TODA INTERVENCIÓN DEBE SER INFORMADA DE INMEDIATO 
+1 Toda OT debe estar firmada por JOP 
+2 Si no esta Jop deben informar de inmediato y enviar imagen de la OT 
+3 La visita debe contar con todos los respaldos de imágenes antes de la intervención del técnico y posterior, además de imágenes de estado de los accesorios 
+4 Ante inconvenientes con chapa randomica, se debe dar aviso inmediato para que Base Santiago pueda enviar a sucursal esta chapa (no es responsabilidad de Position) 
+5 Solo se efectuara asistencia de los móviles que se encuentren en la sucursal respetando los días de visita 
+6 Se debe confirmar con JOP (correo) los datos del técnico que asistirá a la base (patente, nombre completo, Rut) 
+7 Si técnico es externo deben enviar a Mardem bajo mismo correo los antecedentes del técnico para su aprobación. 
+8 Ante inconveniente de acceso, deben informar de inmediato, ya que, correos de accesos son enviados con anticipación. 
+9 Los portátiles se deben posicionar para validar que este funcionando, en caso de tener inconvenientes con el funcionamiento técnico debe traer portátil devuelta y enviar de inmediato para informar a Brinks para su nuevo envío de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Validación I+D 
+1 La validación de la asistencia debe informar motivo de incidencia (falla), en caso que no presente problema debe ser indicado en tkt que se efectuara para la validación. 
+2 Validación MDVR 
+3 Validación Baterías 
+4 Validación Boton Emergencia 
+5 Validación Cyryx 
+6 Validación Caiquen de corresponder 
+7 Validación de GPS 
+8 Validación Cámaras 
+9Validación Monitor 
+10 Valicación Chapa randomica 
+11 Validación boton de MDVR 
+12 Validación grabación de disco duro (debe estar funcional)</t>
+  </si>
+  <si>
+    <t>BRINKS</t>
+  </si>
+  <si>
+    <t>86431800-2</t>
+  </si>
+  <si>
+    <t>SWZK97-MOV23032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARCELO OJEDA </t>
+  </si>
+  <si>
+    <t>MOJEDA@BRINKS.COM</t>
+  </si>
+  <si>
+    <t>AV. PRIETO NORTE 0331, TEMUCO</t>
+  </si>
+  <si>
+    <t>TEMUCO - CAMBIO DE GPS - BRINKS -SVFG59-CB909</t>
+  </si>
+  <si>
+    <t>SVFG59-CB909</t>
+  </si>
+  <si>
+    <t>TEMUCO - CAMBIO DE GPS - BRINKS -RLVL73-MOV19039</t>
+  </si>
+  <si>
+    <t>RLVL73-MOV19039</t>
+  </si>
+  <si>
+    <t>Carlos Ruiz</t>
+  </si>
+  <si>
+    <t>MAIPU- INSTALACIÓN - LUREYE - GENERADOR_SANTIAGO_16</t>
+  </si>
+  <si>
+    <t>Actividad: Instalación 
+Accesorios: GPS 
+Subcuenta de visualización: FLOTA_LUREYE 
+Marca: Sin información 
+Modelo: Sin información 
+Año: Sin informacion</t>
+  </si>
+  <si>
+    <t>Obs I+D: Favor indicar IMEI del dispositivo y nombre que se le colocó</t>
+  </si>
+  <si>
+    <t>Validación KAM: 
+1. actualizar IMEI y nombre en archivo 
+2. Incluir en carpeta respectiva 
+3. formalizar actividad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 18-12-2025 17:06
+COORDINADO DESDE 22.12.25 TECNICO: FABIAN DIAZ
+</t>
+  </si>
+  <si>
+    <t>LUREYE</t>
+  </si>
+  <si>
+    <t>77030540-3</t>
+  </si>
+  <si>
+    <t>GENERADOR_SANTIAGO_16</t>
+  </si>
+  <si>
+    <t>xaviera.gatica@lureye.cl</t>
+  </si>
+  <si>
+    <t>XAVIERA GATICA</t>
+  </si>
+  <si>
+    <t>AV. LO ESPEJO 1300, MAIPU</t>
+  </si>
+  <si>
+    <t>MAIPU</t>
   </si>
   <si>
     <t>AGRETRANS LOA</t>
@@ -305,12 +442,6 @@
   </si>
   <si>
     <t>CALAMA - INSTALACION MVDR4 IA + DMS + ADAS + CAMARA V4 - AGRETRANS - X</t>
-  </si>
-  <si>
-    <t>MDVR 4ch con IA, DMS, ADAS</t>
-  </si>
-  <si>
-    <t>CALAMA - INSTALACION MVDR4 IA + DMS + ADAS+ CAMARA V4 - AGRETRANS - X</t>
   </si>
 </sst>
 </file>
@@ -1170,11 +1301,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B82D388-9366-481A-8E12-BC3B17FE4142}">
-  <dimension ref="A1:BG5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA97B9A-DEDA-43C5-813B-9DA3D3B30576}">
+  <dimension ref="A1:BG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1367,613 +1498,613 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>42329</v>
+        <v>43003</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="U2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="W2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="X2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="AB2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AC2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AD2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AE2">
         <v>24</v>
       </c>
       <c r="AF2" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AG2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AI2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT2">
+        <v>56996396609</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB2">
+        <v>56996396609</v>
+      </c>
+      <c r="BC2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT2">
-        <v>56993093036</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV2" t="s">
+      <c r="BD2" t="s">
         <v>75</v>
       </c>
-      <c r="AW2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>81</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>75</v>
-      </c>
-      <c r="BB2">
-        <v>56993093036</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>71</v>
-      </c>
       <c r="BE2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BF2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BG2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>42328</v>
+        <v>43001</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U3" t="s">
+        <v>67</v>
+      </c>
+      <c r="V3" t="s">
         <v>87</v>
       </c>
-      <c r="U3" t="s">
-        <v>66</v>
-      </c>
-      <c r="V3" t="s">
-        <v>84</v>
-      </c>
       <c r="W3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="X3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="AB3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AC3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AD3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AE3">
         <v>24</v>
       </c>
       <c r="AF3" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AG3" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AI3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT3">
+        <v>56996396609</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>92</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB3">
+        <v>56996396609</v>
+      </c>
+      <c r="BC3" t="s">
         <v>74</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT3">
-        <v>56993093036</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV3" t="s">
+      <c r="BD3" t="s">
         <v>75</v>
       </c>
-      <c r="AW3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>81</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>75</v>
-      </c>
-      <c r="BB3">
-        <v>56993093036</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>71</v>
-      </c>
       <c r="BE3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BF3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BG3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>42327</v>
+        <v>42999</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="K4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T4" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="U4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="W4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="X4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="AB4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AC4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AD4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AE4">
         <v>24</v>
       </c>
       <c r="AF4" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="AG4" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AI4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT4">
+        <v>56996396609</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>92</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB4">
+        <v>56996396609</v>
+      </c>
+      <c r="BC4" t="s">
         <v>74</v>
       </c>
-      <c r="AJ4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT4">
-        <v>56993093036</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV4" t="s">
+      <c r="BD4" t="s">
         <v>75</v>
       </c>
-      <c r="AW4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>81</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>75</v>
-      </c>
-      <c r="BB4">
-        <v>56993093036</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>71</v>
-      </c>
       <c r="BE4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BF4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BG4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>42326</v>
+        <v>42914</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" t="s">
         <v>66</v>
       </c>
-      <c r="E5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" t="s">
-        <v>65</v>
-      </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T5" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="U5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V5" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="W5" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="X5" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -1982,106 +2113,465 @@
         <v>1</v>
       </c>
       <c r="AA5" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="AB5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AC5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AD5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AE5">
         <v>24</v>
       </c>
       <c r="AF5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>110</v>
+      </c>
+      <c r="BB5">
+        <v>978263964</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>111</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>81</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>42347</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
         <v>78</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" t="s">
+        <v>67</v>
+      </c>
+      <c r="S6" t="s">
+        <v>68</v>
+      </c>
+      <c r="T6" t="s">
+        <v>121</v>
+      </c>
+      <c r="U6" t="s">
+        <v>67</v>
+      </c>
+      <c r="V6" t="s">
+        <v>118</v>
+      </c>
+      <c r="W6" t="s">
+        <v>119</v>
+      </c>
+      <c r="X6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE6">
+        <v>24</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI6" t="s">
         <v>79</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AJ6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT6">
+        <v>56993093036</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>115</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB6">
+        <v>56993093036</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>42346</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" t="s">
         <v>66</v>
       </c>
-      <c r="AI5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK5" t="s">
+      <c r="K7" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" t="s">
+        <v>83</v>
+      </c>
+      <c r="M7" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" t="s">
+        <v>67</v>
+      </c>
+      <c r="P7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" t="s">
+        <v>68</v>
+      </c>
+      <c r="T7" t="s">
+        <v>121</v>
+      </c>
+      <c r="U7" t="s">
+        <v>67</v>
+      </c>
+      <c r="V7" t="s">
+        <v>118</v>
+      </c>
+      <c r="W7" t="s">
+        <v>119</v>
+      </c>
+      <c r="X7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD7" t="s">
         <v>69</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AE7">
+        <v>24</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK7" t="s">
         <v>70</v>
       </c>
-      <c r="AM5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT5">
+      <c r="AL7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT7">
         <v>56993093036</v>
       </c>
-      <c r="AU5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>81</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>75</v>
-      </c>
-      <c r="BB5">
+      <c r="AU7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>115</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB7">
         <v>56993093036</v>
       </c>
-      <c r="BC5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>66</v>
+      <c r="BC7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF7" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BG7" xr:uid="{2DA97B9A-DEDA-43C5-813B-9DA3D3B30576}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Fix Schema Endpoint
</commit_message>
<xml_diff>
--- a/backend/Coordinados (11).xlsx
+++ b/backend/Coordinados (11).xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3CDDCE4-2EC1-4337-BCDA-FEFEEA9A286C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3B46EC4-AD08-436B-9C8B-37E97A88CBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{CFC39CBD-85D8-496E-ADDF-C53937D27CDB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{16E0801B-C8FC-4334-823D-E60C3544E7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinados" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coordinados!$A$1:$BG$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coordinados!$A$1:$BG$5</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="120">
   <si>
     <t>ID</t>
   </si>
@@ -208,6 +208,9 @@
     <t>Sergio Ortiz</t>
   </si>
   <si>
+    <t>Sergio Hernandez</t>
+  </si>
+  <si>
     <t>normal</t>
   </si>
   <si>
@@ -226,222 +229,239 @@
     <t>Instalación</t>
   </si>
   <si>
+    <t>09-10-2025</t>
+  </si>
+  <si>
+    <t>29-12-2025</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t>público</t>
   </si>
   <si>
+    <t>CALAMA - INSTALACIÓN  MDVR4 + IA - DMS -ADAS - CÁMARA LATERAL - CÁMARA TRASERA - TRANSPORTES_FCA - PJJR85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVIDAD: INSTALACIÓN DE IMPLEMENTACIÓN TRANSPORTES FCA, CONSIDERAR LOS SIGUIENTES MATERIALES:  
+1.- MDVR DE 4 CANALES CON IA ACTIVA  
+2.- SIMCAD  BAM ENTEL  
+3.- DISCO DUROS 1 TB 
+4.- ADAS  
+5.- DMS  
+6.- CÁMARA V4 TRASERA  
+7.- CAMARA V5 LATERIAL 
+8.- ADAS Y DMS DEBE QUEDAR CONECTADO A INTERMITENTE. 
+</t>
+  </si>
+  <si>
+    <t>VALIDACIÓN I+D 
+1.- SE DEBEN ACTIVAR TODAS LAS ALARMAS SEGUN LA CÁMARA IMPLEMENTADA (ADAS Y DMS) Y CALIBRACIÓN. 
+2.- INDICAR MODELO DE CAMARAS ENVIADAS A CALAMA (PILAR O DE TABLERO SEGUN EL MODELO QUE APLIQUE 
+3..- INDICAR IMEI INSTALADO // 553072927524 
+4.- FOTOGRAFIAS DE IMPLEMENTACIÓN // OK 
+5.- ADAS Y DMS DEBE QUEDAR CONECTADO A INTERMITENTE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Joaquin Lopez 29-12-2025 17:53
+INST MDVR + ADAS + DMS + CAMARA LATERAL + CAMARA TRASERA
+=-=
+@Soledad Brito 23-12-2025 10:55
+COORDINADO CON LUCIANA SOTIL, DESDE 26.12.25 A LAS 09:00 HRS
+=-=
+@Sergio Ortiz 11-11-2025 10:09
+Favor coordinar actividad 
+=-=
+@Soledad Brito 17-10-2025 15:22
+COORDINADO CON ELSA MIRANDA DESDE 20.10.25 
+</t>
+  </si>
+  <si>
     <t>NO</t>
   </si>
   <si>
+    <t>TRANSPORTES_FCA</t>
+  </si>
+  <si>
+    <t>8468228-4</t>
+  </si>
+  <si>
+    <t>106971</t>
+  </si>
+  <si>
+    <t>PJJR85</t>
+  </si>
+  <si>
     <t>Camión</t>
   </si>
   <si>
     <t>GV310LAU</t>
   </si>
   <si>
-    <t>Antena GPS</t>
+    <t>Instalación ACC</t>
+  </si>
+  <si>
+    <t>administradordecontrato@franciscocayo.cl</t>
+  </si>
+  <si>
+    <t>ELSA MIRANDA</t>
+  </si>
+  <si>
+    <t>FRANCISCO MARTINIC (-22.437049653078066, -68.89590402553648)</t>
+  </si>
+  <si>
+    <t>CALAMA</t>
   </si>
   <si>
     <t>Región de Antofagasta.</t>
   </si>
   <si>
-    <t>TEMUCO</t>
-  </si>
-  <si>
     <t>Región de La Araucanía.</t>
   </si>
   <si>
-    <t xml:space="preserve">Instalación </t>
+    <t>Blanca Acuña</t>
+  </si>
+  <si>
+    <t>urgente</t>
+  </si>
+  <si>
+    <t>23-12-2025</t>
+  </si>
+  <si>
+    <t>ANGOL - INSTALACION GPS -  TRANSURSA - RZWJ15</t>
+  </si>
+  <si>
+    <t>ACTIVIDAD : INSTALACION GPS BASICO 
+Tipo  TRACTOCAMION 
+Marca  SCANIA 
+Modelo  R500A6X2 
+Año  2022 
+Color  ROJO 
+N° Motor  8404578 
+N° Chasis  9BSR6X200 N4015507 
+Procedencia  BRAZIL 
+Fabricante  SCANIA BRAZIL 
+Tipo de sello  SELLO VERDE 
+Combustible  DIESEL</t>
+  </si>
+  <si>
+    <t>I+D 
+COMENTARIOS ACTIVIDAD REALIZADA 
+MAS VALIDACIÓN 
+I+D 
+1.- VALIDAR POSICION DE DISPOSITIVO GPS 
+2.- FOTOGRAFÍA FISICA DE LA UBICACIÓN DEL GPS (DONDE QUEDA INSTALADO) (OBLIGATORIO) 
+3.- FOTOGRAFÍA DE PATENTE INTERVENIDA 
+4.- OT FIRMADA 
+5.- CARGA ZONA Y ALARMA DE VELOCIDAD EN ZONA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 29-12-2025 16:27
+COORDINADO CON CLAUDIO ERICES PARA 30.12.25 A LAS 10.00
+</t>
+  </si>
+  <si>
+    <t>TRANSURSA</t>
+  </si>
+  <si>
+    <t>77218515-4</t>
+  </si>
+  <si>
+    <t>RZWJ15</t>
+  </si>
+  <si>
+    <t>CLAUDIO ERICES RUIZ</t>
+  </si>
+  <si>
+    <t>CALLE RUCAPELLAN 971, ANGOL</t>
+  </si>
+  <si>
+    <t>ANGOL</t>
   </si>
   <si>
     <t>Soporte</t>
   </si>
   <si>
-    <t>Yessica Santibañez</t>
-  </si>
-  <si>
-    <t>PENDIENTE</t>
-  </si>
-  <si>
-    <t>CALLE N°8 SITIO N°6 MZA K SECTOR PUERTO SECO. CALAMA</t>
-  </si>
-  <si>
-    <t>Región Metropolitana de Santiago.</t>
-  </si>
-  <si>
-    <t>18-12-2025</t>
-  </si>
-  <si>
-    <t>10-12-2025</t>
-  </si>
-  <si>
-    <t>Constanza Barrios</t>
-  </si>
-  <si>
-    <t>22-12-2025</t>
-  </si>
-  <si>
-    <t>TEMUCO - CAMBIO DE GPS - BRINKS -SWZK97-MOV23032</t>
-  </si>
-  <si>
-    <t>ACTIVIDAD: CAMBIO DE GPS  
-TODA INTERVENCIÓN DEBE SER INFORMADA DE INMEDIATO 
-1 Toda OT debe estar firmada por JOP 
-2 Si no esta Jop deben informar de inmediato y enviar imagen de la OT 
-3 La visita debe contar con todos los respaldos de imágenes antes de la intervención del técnico y posterior, además de imágenes de estado de los accesorios 
-4 Ante inconvenientes con chapa randomica, se debe dar aviso inmediato para que Base Santiago pueda enviar a sucursal esta chapa (no es responsabilidad de Position) 
-5 Solo se efectuara asistencia de los móviles que se encuentren en la sucursal respetando los días de visita 
-6 Se debe confirmar con JOP (correo) los datos del técnico que asistirá a la base (patente, nombre completo, Rut) 
-7 Si técnico es externo deben enviar a Mardem bajo mismo correo los antecedentes del técnico para su aprobación. 
-8 Ante inconveniente de acceso, deben informar de inmediato, ya que, correos de accesos son enviados con anticipación. 
-9 Los portátiles se deben posicionar para validar que este funcionando, en caso de tener inconvenientes con el funcionamiento técnico debe traer portátil devuelta y enviar de inmediato para informar a Brinks para su nuevo envío de</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Validación I+D 
-1 La validación de la asistencia debe informar motivo de incidencia (falla), en caso que no presente problema debe ser indicado en tkt que se efectuara para la validación. 
-2 Validación MDVR 
-3 Validación Baterías 
-4 Validación Boton Emergencia 
-5 Validación Cyryx 
-6 Validación Caiquen de corresponder 
-7 Validación de GPS 
-8 Validación Cámaras 
-9Validación Monitor 
-10 Valicación Chapa randomica 
-11 Validación boton de MDVR 
-12 Validación grabación de disco duro (debe estar funcional)</t>
-  </si>
-  <si>
-    <t>BRINKS</t>
-  </si>
-  <si>
-    <t>86431800-2</t>
-  </si>
-  <si>
-    <t>SWZK97-MOV23032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARCELO OJEDA </t>
-  </si>
-  <si>
-    <t>MOJEDA@BRINKS.COM</t>
-  </si>
-  <si>
-    <t>AV. PRIETO NORTE 0331, TEMUCO</t>
-  </si>
-  <si>
-    <t>TEMUCO - CAMBIO DE GPS - BRINKS -SVFG59-CB909</t>
-  </si>
-  <si>
-    <t>SVFG59-CB909</t>
-  </si>
-  <si>
-    <t>TEMUCO - CAMBIO DE GPS - BRINKS -RLVL73-MOV19039</t>
-  </si>
-  <si>
-    <t>RLVL73-MOV19039</t>
-  </si>
-  <si>
-    <t>Carlos Ruiz</t>
-  </si>
-  <si>
-    <t>MAIPU- INSTALACIÓN - LUREYE - GENERADOR_SANTIAGO_16</t>
-  </si>
-  <si>
-    <t>Actividad: Instalación 
-Accesorios: GPS 
-Subcuenta de visualización: FLOTA_LUREYE 
-Marca: Sin información 
-Modelo: Sin información 
-Año: Sin informacion</t>
-  </si>
-  <si>
-    <t>Obs I+D: Favor indicar IMEI del dispositivo y nombre que se le colocó</t>
-  </si>
-  <si>
-    <t>Validación KAM: 
-1. actualizar IMEI y nombre en archivo 
-2. Incluir en carpeta respectiva 
-3. formalizar actividad.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 18-12-2025 17:06
-COORDINADO DESDE 22.12.25 TECNICO: FABIAN DIAZ
-</t>
-  </si>
-  <si>
-    <t>LUREYE</t>
-  </si>
-  <si>
-    <t>77030540-3</t>
-  </si>
-  <si>
-    <t>GENERADOR_SANTIAGO_16</t>
-  </si>
-  <si>
-    <t>xaviera.gatica@lureye.cl</t>
-  </si>
-  <si>
-    <t>XAVIERA GATICA</t>
-  </si>
-  <si>
-    <t>AV. LO ESPEJO 1300, MAIPU</t>
-  </si>
-  <si>
-    <t>MAIPU</t>
-  </si>
-  <si>
-    <t>AGRETRANS LOA</t>
-  </si>
-  <si>
-    <t>75584300-8</t>
-  </si>
-  <si>
-    <t>MDVR 4ch con IA, V4, DMS, ADAS</t>
-  </si>
-  <si>
-    <t>CARLOS ORTEGA</t>
-  </si>
-  <si>
-    <t>administrador.dch@agretrans.cl</t>
-  </si>
-  <si>
-    <t>26-11-2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVIDAD: MVDR4 + DMS + ADAS 
-Patente  
-Tipo TRACTOCAMION 
-Marca  
-Modelo  
-Año  
-Color  
-N° Motor </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   I+D 
+    <t>26-12-2025</t>
+  </si>
+  <si>
+    <t>CALAMA - REVISION DASHCAM  ADAS+ DMS - TMICHEA - LXWK57</t>
+  </si>
+  <si>
+    <t>ACTIVIDAD: REVISION DASHCAM ADAS ACTIVADO + DMS (SIN TRANSMITIR 23-11-24) 
+Tipo  TRACTOCAMION 
+Marca  VOLVO 
+Modelo  FH 
+Año  2020 
+Color  BLANCO 
+N° Motor  D138033501C4E 
+N° Chasis  9BVRG20C0LE878437 
+Procedencia  BRAZIL 
+Fabricante  VOLVO TRUCKS 
+Tipo de sello  SELLO VERDE 
+Combustible  DIESEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    I+D 
 Favor validar correcto funcionamiento 
-1.- Validación transmisión GPS y latencia cada 30 seg 
-2.- Cargar zona y alarmas accesorios 
-3.- Validación accesorios en Plataforma 
-4.- funcionamiento inteligencia artificial mas calibración 
-5.- validar inteligencia artificial modulo evidencia, Ojos cerrados, uso de telefono (VSS) 
-6.- MVDR debe entregar posicionamiento (VALIDAR SATELITES) 
-7.- validar transmisión en línea de cámaras 
+1.- funcionamiento inteligencia artificial mas calibración 
+2.- validar inteligencia artificial modulo evidencia (VSS  (modulo evidencia, llamada, ojos cerrado, bostezo, etc) )) 
+3.- DASHCAM debe entregar posicionamiento (VALIDAR SATELITES) 
+4.- validar transmisión en línea de cámaras 
+5.- validar correcto funcionamiento GPS 
+6.- validar correcto funcionamiento Ibutton con corte mas buzzer (validar en plataforma) 
+7.- De encontrar intervención o cámara movida adjuntar fotografía 
 8.- fotografía de Disco duro 
 9.- Respaldo OT 
-10.-Conectar a intermitentes 
-11.- SIMCARD CLARO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 10-12-2025 17:10
-COORDINADO DESDE 11.12.25 TECNICO: ORLANDO LUGO
+10.-Integración wisetrack: latencia cada 3 seg, + sensibilidad 3 ejes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 29-12-2025 16:10
+COORDINADO CON SEBASTIAN CARRIZO PARA 30.12.25 A LAS 10:30 HRS
+=-=
+@Blanca Acuña 29-12-2025 16:00
+Estimados estado de coordinación, cliente se encuentra consultando
 </t>
   </si>
   <si>
-    <t>CALAMA - INSTALACION MVDR4 IA + DMS + ADAS + CAMARA V4 - AGRETRANS - X</t>
+    <t>TRANS_MICHEA</t>
+  </si>
+  <si>
+    <t>76662759-5</t>
+  </si>
+  <si>
+    <t>LXWK57</t>
+  </si>
+  <si>
+    <t>Rampla</t>
+  </si>
+  <si>
+    <t>SEBASTIAN CARRIZO</t>
+  </si>
+  <si>
+    <t>PUERTO SECO RUTA CHIU CHIU, CALLE INTERIOR LOTE B, Sitio 20</t>
+  </si>
+  <si>
+    <t>CALAMA - REVISION SENSOR RETROCESO - TMICHEA - PXKT71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVIDAD: REVISION SENSOR RETROCESO CLIENTE INDICA QUE NO ESTA FUNCIONANDO 
+Tipo  SEMIREMOLQUE 
+Marca  RANDON 
+</t>
+  </si>
+  <si>
+    <t>I+D 
+1.- VALIDAR FUNCIONAMIENTO SENSOR RETROCESO 
+2. FOTOGRAFIAS UNIDAD INTERVENIDA 
+3.- DE EXISTIR DAÑOS ADJUNTAR IMAGEN ANTES Y POSTERIOR.</t>
+  </si>
+  <si>
+    <t>PXKT71</t>
+  </si>
+  <si>
+    <t>GPS</t>
   </si>
 </sst>
 </file>
@@ -1301,11 +1321,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA97B9A-DEDA-43C5-813B-9DA3D3B30576}">
-  <dimension ref="A1:BG7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B432B93C-6FCD-4719-AF7A-CBEF1073223D}">
+  <dimension ref="A1:BG5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1498,1080 +1518,722 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>43003</v>
+        <v>40425</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" t="s">
-        <v>77</v>
-      </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="M2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="R2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="T2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="U2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="V2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="W2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="X2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="AB2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AC2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="AE2">
         <v>24</v>
       </c>
       <c r="AF2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="AG2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AI2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="AJ2" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="AK2" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="AL2" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="AM2" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="AN2" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AO2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AP2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AQ2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AR2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AS2" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="AT2">
-        <v>56996396609</v>
+        <v>0</v>
       </c>
       <c r="AU2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="AV2" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="AW2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AX2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AY2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AZ2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="BA2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="BB2">
-        <v>56996396609</v>
+        <v>942206090</v>
       </c>
       <c r="BC2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="BD2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="BE2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="BF2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="BG2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>43001</v>
+        <v>43019</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>77</v>
-      </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="L3" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="M3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="P3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="R3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="S3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="T3" t="s">
+        <v>93</v>
+      </c>
+      <c r="U3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" t="s">
+        <v>70</v>
+      </c>
+      <c r="X3" t="s">
         <v>95</v>
-      </c>
-      <c r="U3" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" t="s">
-        <v>87</v>
-      </c>
-      <c r="W3" t="s">
-        <v>88</v>
-      </c>
-      <c r="X3" t="s">
-        <v>67</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="AB3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AC3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="AE3">
         <v>24</v>
       </c>
       <c r="AF3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>101</v>
+      </c>
+      <c r="BB3">
+        <v>977060355</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>102</v>
+      </c>
+      <c r="BD3" t="s">
         <v>89</v>
       </c>
-      <c r="AG3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>96</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT3">
-        <v>56996396609</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>92</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>94</v>
-      </c>
-      <c r="BB3">
-        <v>56996396609</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>74</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>75</v>
-      </c>
       <c r="BE3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="BF3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="BG3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>42999</v>
+        <v>43528</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="L4" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="M4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="P4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="R4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="S4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="T4" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="U4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="V4" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="W4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="X4" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA4" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="AB4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AC4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD4" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="AE4">
         <v>24</v>
       </c>
       <c r="AF4" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="AG4" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="AH4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AI4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AJ4" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="AK4" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="AL4" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="AM4" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="AN4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AO4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AP4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AQ4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AR4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AS4" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="AT4">
-        <v>56996396609</v>
+        <v>0</v>
       </c>
       <c r="AU4" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="AV4" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="AW4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AX4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AY4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AZ4" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="BA4" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="BB4">
-        <v>56996396609</v>
+        <v>934118075</v>
       </c>
       <c r="BC4" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="BD4" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="BE4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="BF4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="BG4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>42914</v>
+        <v>43527</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="K5" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="L5" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="M5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="N5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="P5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="R5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="S5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="T5" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="U5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="V5" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="W5" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="X5" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="Y5">
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="AB5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AC5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AD5" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="AE5">
         <v>24</v>
       </c>
       <c r="AF5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AG5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="AH5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AI5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AJ5" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="AK5" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="AL5" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="AM5" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="AN5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AO5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AP5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AQ5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AR5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AS5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AT5">
         <v>0</v>
       </c>
       <c r="AU5" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="AV5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AW5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AX5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AY5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AZ5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="BA5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="BB5">
-        <v>978263964</v>
+        <v>934118075</v>
       </c>
       <c r="BC5" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="BD5" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="BE5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="BF5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="BG5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>42347</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L6" t="s">
-        <v>83</v>
-      </c>
-      <c r="M6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" t="s">
-        <v>67</v>
-      </c>
-      <c r="P6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>67</v>
-      </c>
-      <c r="R6" t="s">
-        <v>67</v>
-      </c>
-      <c r="S6" t="s">
-        <v>68</v>
-      </c>
-      <c r="T6" t="s">
-        <v>121</v>
-      </c>
-      <c r="U6" t="s">
-        <v>67</v>
-      </c>
-      <c r="V6" t="s">
-        <v>118</v>
-      </c>
-      <c r="W6" t="s">
-        <v>119</v>
-      </c>
-      <c r="X6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>1</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE6">
-        <v>24</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>115</v>
-      </c>
-      <c r="AT6">
-        <v>56993093036</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>115</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB6">
-        <v>56993093036</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>67</v>
-      </c>
-      <c r="BD6" t="s">
-        <v>73</v>
-      </c>
-      <c r="BE6" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF6" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>42346</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" t="s">
-        <v>117</v>
-      </c>
-      <c r="L7" t="s">
-        <v>83</v>
-      </c>
-      <c r="M7" t="s">
-        <v>67</v>
-      </c>
-      <c r="N7" t="s">
-        <v>67</v>
-      </c>
-      <c r="O7" t="s">
-        <v>67</v>
-      </c>
-      <c r="P7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>67</v>
-      </c>
-      <c r="R7" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" t="s">
-        <v>68</v>
-      </c>
-      <c r="T7" t="s">
-        <v>121</v>
-      </c>
-      <c r="U7" t="s">
-        <v>67</v>
-      </c>
-      <c r="V7" t="s">
-        <v>118</v>
-      </c>
-      <c r="W7" t="s">
-        <v>119</v>
-      </c>
-      <c r="X7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>1</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE7">
-        <v>24</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>115</v>
-      </c>
-      <c r="AT7">
-        <v>56993093036</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>116</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>115</v>
-      </c>
-      <c r="BA7" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB7">
-        <v>56993093036</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>67</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>73</v>
-      </c>
-      <c r="BE7" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF7" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BG7" xr:uid="{2DA97B9A-DEDA-43C5-813B-9DA3D3B30576}"/>
+  <autoFilter ref="A1:BG5" xr:uid="{B432B93C-6FCD-4719-AF7A-CBEF1073223D}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: Enforce Points Rules (Signed Only + Success Only)
</commit_message>
<xml_diff>
--- a/backend/Coordinados (11).xlsx
+++ b/backend/Coordinados (11).xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3B46EC4-AD08-436B-9C8B-37E97A88CBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B9A4848-D422-41D1-9E87-175B5229ACE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{16E0801B-C8FC-4334-823D-E60C3544E7ED}"/>
+    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{132236D4-E3B4-4A87-BB26-8ED1548DC6E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinados" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coordinados!$A$1:$BG$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coordinados!$A$1:$BG$125</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -208,9 +208,6 @@
     <t>Sergio Ortiz</t>
   </si>
   <si>
-    <t>Sergio Hernandez</t>
-  </si>
-  <si>
     <t>normal</t>
   </si>
   <si>
@@ -229,10 +226,7 @@
     <t>Instalación</t>
   </si>
   <si>
-    <t>09-10-2025</t>
-  </si>
-  <si>
-    <t>29-12-2025</t>
+    <t>30-12-2025</t>
   </si>
   <si>
     <t/>
@@ -241,227 +235,254 @@
     <t>público</t>
   </si>
   <si>
-    <t>CALAMA - INSTALACIÓN  MDVR4 + IA - DMS -ADAS - CÁMARA LATERAL - CÁMARA TRASERA - TRANSPORTES_FCA - PJJR85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVIDAD: INSTALACIÓN DE IMPLEMENTACIÓN TRANSPORTES FCA, CONSIDERAR LOS SIGUIENTES MATERIALES:  
-1.- MDVR DE 4 CANALES CON IA ACTIVA  
-2.- SIMCAD  BAM ENTEL  
-3.- DISCO DUROS 1 TB 
-4.- ADAS  
-5.- DMS  
-6.- CÁMARA V4 TRASERA  
-7.- CAMARA V5 LATERIAL 
-8.- ADAS Y DMS DEBE QUEDAR CONECTADO A INTERMITENTE. 
+    <t>NO</t>
+  </si>
+  <si>
+    <t>GV310LAU</t>
+  </si>
+  <si>
+    <t>Región Metropolitana de Santiago.</t>
+  </si>
+  <si>
+    <t>Soporte</t>
+  </si>
+  <si>
+    <t>24-12-2025</t>
+  </si>
+  <si>
+    <t>TEMUCO</t>
+  </si>
+  <si>
+    <t>Región de La Araucanía.</t>
+  </si>
+  <si>
+    <t>Arriendo</t>
+  </si>
+  <si>
+    <t>Camión</t>
+  </si>
+  <si>
+    <t>TEMUCO - INSTALACIÓN GPS + ACCESORIOS - DIWATTS - TRPT29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad: Instalación 
+Accesorios: GPS, Corte de motor, Sonda de temperatura y Sensor de puertas  
+Subcuenta de visualización: WATTS2 
+Marca: Hino 
+Modelo: XZU 917 
+Año: 2025 
+Obs: Favor coordinar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 30-12-2025 16:57
+COORDINADO CON MAGDALENA PONCE, PARA 05.01.25
+=-=
+@Soledad Brito 30-12-2025 16:05
+MAGDALENA PONCE, REVISARÁ RUTA Y DEVOLVERÁ EL LLAMADO
 </t>
   </si>
   <si>
-    <t>VALIDACIÓN I+D 
-1.- SE DEBEN ACTIVAR TODAS LAS ALARMAS SEGUN LA CÁMARA IMPLEMENTADA (ADAS Y DMS) Y CALIBRACIÓN. 
-2.- INDICAR MODELO DE CAMARAS ENVIADAS A CALAMA (PILAR O DE TABLERO SEGUN EL MODELO QUE APLIQUE 
-3..- INDICAR IMEI INSTALADO // 553072927524 
-4.- FOTOGRAFIAS DE IMPLEMENTACIÓN // OK 
-5.- ADAS Y DMS DEBE QUEDAR CONECTADO A INTERMITENTE.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Joaquin Lopez 29-12-2025 17:53
-INST MDVR + ADAS + DMS + CAMARA LATERAL + CAMARA TRASERA
+    <t>DIWATTS</t>
+  </si>
+  <si>
+    <t>76455830-8</t>
+  </si>
+  <si>
+    <t>TRPT29</t>
+  </si>
+  <si>
+    <t>magdalena.ponce@watts.cl</t>
+  </si>
+  <si>
+    <t>MAGDALENA PONCE</t>
+  </si>
+  <si>
+    <t>PANAMERICANA SUR KM. 678 PADRE LAS CASAS</t>
+  </si>
+  <si>
+    <t>Blanca Acuña</t>
+  </si>
+  <si>
+    <t>27-11-2025</t>
+  </si>
+  <si>
+    <t>CHILLAN - INSTALACIÓN GPS - ACCESORIOS - CIAL_ALIMENTOS - VE839-POR CONFIRMAR</t>
+  </si>
+  <si>
+    <t>ACTIVIDAD: INSTALACIÓN  
+GPS  
+BOTON EMERGENCIA  
+CORTE MOTOR  
+SENSOR DE TEMPERATURA CON DOBLE SONDA 
+2 SENSOR MAGNETICO 
+RETIRO EQUIPO COMPETENCIA  
+Información vehicular 
+VEHICULO NUEVO DISPONIBLE A PARTIR DE LA SEMANA 08/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALIDACIÓN I+D  
+1.- VALIDAR POSICION DE DISPOSITIVO GPS  
+2.- VALIDACIÓN DE FUNCIONAMIENTO BOTON EMERGENCIA  
+3.- VALIDACIÓN DE FUNCIONAMIENTO CORTE MOTOR  
+4.- VALIDACIÓN DE FUNCIONAMIENTO SENSOR PUERTA  
+5.- VALIDACIÓN DE SENSOR DE TEMPERATURA (AMBAS SONDAS DEBEN ESTAR FUNCIONALES) 
+6.- FOTOGRAFIA DE GPS COMPETENCIA (NUMERO DE SERIE)  
+7.- FOTOGRAFÍA FISICA DE LA UBICACIÓN DEL GPS (DONDE QUEDA INSTALADO) (OBLIGATORIO) 
+8.- FOTOGRAFÍA DE PATENTE INTERVENIDA  
+9.- OT FIRMADA  
+10.- DAR VISUALIZACIÓN A SUBCUENTA FLOTA_CIALALIMENTOS 
+ZONA Y ALARMA  
+1.- VELOCIDAD 95 KM POR 1 MINUTO  
+2.- CARGA DE ZONAS POR ACCESORIOS IMPLEMENTADOS  
+3.- CARGAR ALARMA DE TEMPERATURA PEGADA  
+4.- SIN COBERTURA GPS  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 30-12-2025 16:55
+RECOORDINADO CON HECTOR CORREA, PARA 08-01-25 A LAS 15:00 HRS
 =-=
-@Soledad Brito 23-12-2025 10:55
-COORDINADO CON LUCIANA SOTIL, DESDE 26.12.25 A LAS 09:00 HRS
+@Blanca Acuña 30-12-2025 16:39
+Estimados favor proceder con coordinación, cliente cuenta con unidad disponible
 =-=
-@Sergio Ortiz 11-11-2025 10:09
-Favor coordinar actividad 
+@Soledad Brito 15-12-2025 10:33
+COORDINADO CON HECTOR CORREA, PARA 18.12.25 A LAS 14:00 HRS.
 =-=
-@Soledad Brito 17-10-2025 15:22
-COORDINADO CON ELSA MIRANDA DESDE 20.10.25 
+@Soledad Brito 09-12-2025 17:22
+HECTOR CORREA, CONFIRMARÁ SI PODEMOS REALIZAR LA INSTALACIÓN 10.12.25,
+=-=
+@Nicolas del Rio 05-12-2025 13:21
+ESTIMADOS 
+JUNTO CON SALUDAR. 
+CLIENTE SEÑALA QUE HAY QUE LLAMARLO SEMANA DEL 8 DICIEMBRE PARA VER SI ESTA DISPONIBLE EL NUEVO VEHICULO. 
+GRACIAS 
+SALUDOS
+=-=
+@Nicolas del Rio 03-12-2025 17:40
+ESTIMADAS/OS 
+JUNTO CON SALUDAR, VEHICULO PENDIENTE DE CONFIRMACION POR JO CIAL CHILLAN. 
+FAVOR CUANDO ESTE OK LA SOLICITUD DEL CLIENTE, ENTREGAR A OPERACIONES PARA COORDINAR. 
+QUEDO ATENTO A DUDAS. 
+SALUDOS
+=-=
+@Soledad Brito 01-12-2025 10:27
+COORDINADO PARA 01.12.25 A LAS 13:00 HRS.
+=-=
+@Soledad Brito 28-11-2025 18:08
+HECTOR CORREA INDICA QUE DEVOLVERÁ EL LLAMADO
+=-=
+@Blanca Acuña 27-11-2025 17:03
+Estimada este es el nuevo TKT ya que se mantiene numero interno
+=-=
+@Soledad Brito 27-11-2025 15:47
+POR FAVOR REVISAR QUE PATENTE INSTALARAN EN LUGAR DE ESTA
 </t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>TRANSPORTES_FCA</t>
-  </si>
-  <si>
-    <t>8468228-4</t>
-  </si>
-  <si>
-    <t>106971</t>
-  </si>
-  <si>
-    <t>PJJR85</t>
-  </si>
-  <si>
-    <t>Camión</t>
-  </si>
-  <si>
-    <t>GV310LAU</t>
-  </si>
-  <si>
-    <t>Instalación ACC</t>
-  </si>
-  <si>
-    <t>administradordecontrato@franciscocayo.cl</t>
-  </si>
-  <si>
-    <t>ELSA MIRANDA</t>
-  </si>
-  <si>
-    <t>FRANCISCO MARTINIC (-22.437049653078066, -68.89590402553648)</t>
-  </si>
-  <si>
-    <t>CALAMA</t>
-  </si>
-  <si>
-    <t>Región de Antofagasta.</t>
-  </si>
-  <si>
-    <t>Región de La Araucanía.</t>
-  </si>
-  <si>
-    <t>Blanca Acuña</t>
-  </si>
-  <si>
-    <t>urgente</t>
-  </si>
-  <si>
-    <t>23-12-2025</t>
-  </si>
-  <si>
-    <t>ANGOL - INSTALACION GPS -  TRANSURSA - RZWJ15</t>
-  </si>
-  <si>
-    <t>ACTIVIDAD : INSTALACION GPS BASICO 
-Tipo  TRACTOCAMION 
-Marca  SCANIA 
-Modelo  R500A6X2 
-Año  2022 
-Color  ROJO 
-N° Motor  8404578 
-N° Chasis  9BSR6X200 N4015507 
-Procedencia  BRAZIL 
-Fabricante  SCANIA BRAZIL 
-Tipo de sello  SELLO VERDE 
-Combustible  DIESEL</t>
-  </si>
-  <si>
-    <t>I+D 
-COMENTARIOS ACTIVIDAD REALIZADA 
-MAS VALIDACIÓN 
-I+D 
-1.- VALIDAR POSICION DE DISPOSITIVO GPS 
-2.- FOTOGRAFÍA FISICA DE LA UBICACIÓN DEL GPS (DONDE QUEDA INSTALADO) (OBLIGATORIO) 
-3.- FOTOGRAFÍA DE PATENTE INTERVENIDA 
-4.- OT FIRMADA 
-5.- CARGA ZONA Y ALARMA DE VELOCIDAD EN ZONA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 29-12-2025 16:27
-COORDINADO CON CLAUDIO ERICES PARA 30.12.25 A LAS 10.00
+    <t>CIAL_ALIMENTOS</t>
+  </si>
+  <si>
+    <t>80186300-0</t>
+  </si>
+  <si>
+    <t>VE839-POR CONFIRMAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalación </t>
+  </si>
+  <si>
+    <t>HECTOR CORREA</t>
+  </si>
+  <si>
+    <t>RUTA 5 SUR KM 8 SN</t>
+  </si>
+  <si>
+    <t>CHILLAN</t>
+  </si>
+  <si>
+    <t>Región del Ñuble.</t>
+  </si>
+  <si>
+    <t>SAN BERNARDO - REVISIÓN GPS - CUENTA_CAROZZIDISTRIBUCION - HLPX63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad: Revisión 
+Accesorios: GPS  
+Año GPS: GV310LAU 2024 
+Marca: Sinotruck 
+Modelo: TR 420 
+Año: 2016 
+Obs: Revisar, presenta exceso de saltos de posición. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 30-12-2025 16:49
+COORDINADO CON CHRISTOPHER AGURTO PARA 31.12.25 A LAS 10:00 HRS
+=-=
+@Soledad Brito 30-12-2025 10:52
+CHRISTOPHER AGURTO, REVISARÁ RUTA Y DEVOLVERÁ EL LLAMADO
 </t>
   </si>
   <si>
-    <t>TRANSURSA</t>
-  </si>
-  <si>
-    <t>77218515-4</t>
-  </si>
-  <si>
-    <t>RZWJ15</t>
-  </si>
-  <si>
-    <t>CLAUDIO ERICES RUIZ</t>
-  </si>
-  <si>
-    <t>CALLE RUCAPELLAN 971, ANGOL</t>
-  </si>
-  <si>
-    <t>ANGOL</t>
-  </si>
-  <si>
-    <t>Soporte</t>
-  </si>
-  <si>
-    <t>26-12-2025</t>
-  </si>
-  <si>
-    <t>CALAMA - REVISION DASHCAM  ADAS+ DMS - TMICHEA - LXWK57</t>
-  </si>
-  <si>
-    <t>ACTIVIDAD: REVISION DASHCAM ADAS ACTIVADO + DMS (SIN TRANSMITIR 23-11-24) 
-Tipo  TRACTOCAMION 
-Marca  VOLVO 
-Modelo  FH 
-Año  2020 
-Color  BLANCO 
-N° Motor  D138033501C4E 
-N° Chasis  9BVRG20C0LE878437 
-Procedencia  BRAZIL 
-Fabricante  VOLVO TRUCKS 
-Tipo de sello  SELLO VERDE 
-Combustible  DIESEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    I+D 
-Favor validar correcto funcionamiento 
-1.- funcionamiento inteligencia artificial mas calibración 
-2.- validar inteligencia artificial modulo evidencia (VSS  (modulo evidencia, llamada, ojos cerrado, bostezo, etc) )) 
-3.- DASHCAM debe entregar posicionamiento (VALIDAR SATELITES) 
-4.- validar transmisión en línea de cámaras 
-5.- validar correcto funcionamiento GPS 
-6.- validar correcto funcionamiento Ibutton con corte mas buzzer (validar en plataforma) 
-7.- De encontrar intervención o cámara movida adjuntar fotografía 
-8.- fotografía de Disco duro 
-9.- Respaldo OT 
-10.-Integración wisetrack: latencia cada 3 seg, + sensibilidad 3 ejes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 29-12-2025 16:10
-COORDINADO CON SEBASTIAN CARRIZO PARA 30.12.25 A LAS 10:30 HRS
+    <t>CUENTA_CAROZZIDISTRIBUCION</t>
+  </si>
+  <si>
+    <t>96591040-9</t>
+  </si>
+  <si>
+    <t>46406</t>
+  </si>
+  <si>
+    <t>HLPX63</t>
+  </si>
+  <si>
+    <t>christopher.agurto@carozzi.cl</t>
+  </si>
+  <si>
+    <t>CHRISTOPHER AGURTO</t>
+  </si>
+  <si>
+    <t>CAMINO LONGITUDINAL SUR 5201, NOS</t>
+  </si>
+  <si>
+    <t>SAN BERNARDO</t>
+  </si>
+  <si>
+    <t>TEMUCO - CAMBIO GPS + VALIDACIÓN - CUENTA_CAROZZIDISTRIBUCION - BWYY79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVIDAD: CAMBIO GPS +VALIDACIÓN ENTEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 30-12-2025 13:01
+PEDRO BUSTAMANTE, CELULAR CORRECTO ES +56971869734 X FAVOAR EDITAR, COORDINADO PARA 10.01.26 A LAS 09:00 
 =-=
-@Blanca Acuña 29-12-2025 16:00
-Estimados estado de coordinación, cliente se encuentra consultando
+@Soledad Brito 30-12-2025 12:55
+PEDRO BUSTAMANTE, INDICA QUE ESTÁN CON MUCHO TRABAJO, QUE TIENEN DISPONIBILIDAD PARA DÍA SABADO 10.01.25 A LAS 09:00 SE ENVIA CORREO CON PROGRAMACIÓN
 </t>
   </si>
   <si>
-    <t>TRANS_MICHEA</t>
-  </si>
-  <si>
-    <t>76662759-5</t>
-  </si>
-  <si>
-    <t>LXWK57</t>
-  </si>
-  <si>
-    <t>Rampla</t>
-  </si>
-  <si>
-    <t>SEBASTIAN CARRIZO</t>
-  </si>
-  <si>
-    <t>PUERTO SECO RUTA CHIU CHIU, CALLE INTERIOR LOTE B, Sitio 20</t>
-  </si>
-  <si>
-    <t>CALAMA - REVISION SENSOR RETROCESO - TMICHEA - PXKT71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVIDAD: REVISION SENSOR RETROCESO CLIENTE INDICA QUE NO ESTA FUNCIONANDO 
-Tipo  SEMIREMOLQUE 
-Marca  RANDON 
-</t>
-  </si>
-  <si>
-    <t>I+D 
-1.- VALIDAR FUNCIONAMIENTO SENSOR RETROCESO 
-2. FOTOGRAFIAS UNIDAD INTERVENIDA 
-3.- DE EXISTIR DAÑOS ADJUNTAR IMAGEN ANTES Y POSTERIOR.</t>
-  </si>
-  <si>
-    <t>PXKT71</t>
+    <t>19331</t>
+  </si>
+  <si>
+    <t>BWYY79</t>
+  </si>
+  <si>
+    <t>pedro.bustamante@carozzi.cl</t>
+  </si>
+  <si>
+    <t>PEDRO BUSTAMANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUIDO BECK DE RAMBERGA 1884, PADRE DE LAS CASAS </t>
   </si>
   <si>
     <t>GPS</t>
+  </si>
+  <si>
+    <t>GPS, Corta Corriente, Sensor Pta, Sensor Temperatura</t>
+  </si>
+  <si>
+    <t>GPS, Botón Alámbrico Tablero, Corta Corriente, Sensor Pta, Sensor Pta Adicional, Sensor Temperatura, Sensor Temperatura Adicional</t>
   </si>
 </sst>
 </file>
@@ -604,7 +625,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -782,6 +803,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -945,8 +972,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -992,7 +1023,24 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1321,23 +1369,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B432B93C-6FCD-4719-AF7A-CBEF1073223D}">
-  <dimension ref="A1:BG5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9B5D47-907A-40D6-BA1C-6246DAD5644F}">
+  <dimension ref="A1:BG125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.53125" customWidth="1"/>
-    <col min="25" max="26" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.46484375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.06640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="114.53125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="255.59765625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="255.59765625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.53125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.06640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="109.1328125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="36.06640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="50.9296875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.86328125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="59.53125" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="41.73046875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1516,9 +1614,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>40425</v>
+        <v>43572</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
@@ -1527,604 +1625,604 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
         <v>61</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>63</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>64</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>65</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>66</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>67</v>
       </c>
-      <c r="K2" t="s">
-        <v>68</v>
-      </c>
       <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" t="s">
         <v>69</v>
       </c>
-      <c r="M2" t="s">
+      <c r="T2" t="s">
+        <v>79</v>
+      </c>
+      <c r="U2" t="s">
+        <v>68</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W2" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" t="s">
         <v>70</v>
-      </c>
-      <c r="N2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" t="s">
-        <v>70</v>
-      </c>
-      <c r="P2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W2" t="s">
-        <v>74</v>
-      </c>
-      <c r="X2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y2">
-        <v>9</v>
-      </c>
-      <c r="Z2">
-        <v>4</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>76</v>
       </c>
       <c r="AE2">
         <v>24</v>
       </c>
       <c r="AF2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" t="s">
         <v>77</v>
       </c>
-      <c r="AG2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>70</v>
-      </c>
       <c r="AI2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="AJ2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AK2" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="AL2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>119</v>
+        <v>71</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="AN2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="AO2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AP2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AQ2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AR2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AS2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AT2">
         <v>0</v>
       </c>
       <c r="AU2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AV2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AW2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AX2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AY2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AZ2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="BA2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BB2">
-        <v>942206090</v>
+        <v>972173626</v>
       </c>
       <c r="BC2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="BD2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="BE2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BF2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BG2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>43019</v>
+        <v>42426</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
       <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>68</v>
+      </c>
+      <c r="R3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" t="s">
+      <c r="U3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>10</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD3" t="s">
         <v>70</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" t="s">
-        <v>92</v>
-      </c>
-      <c r="L3" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" t="s">
-        <v>70</v>
-      </c>
-      <c r="O3" t="s">
-        <v>70</v>
-      </c>
-      <c r="P3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" t="s">
-        <v>70</v>
-      </c>
-      <c r="S3" t="s">
-        <v>71</v>
-      </c>
-      <c r="T3" t="s">
-        <v>93</v>
-      </c>
-      <c r="U3" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3" t="s">
-        <v>94</v>
-      </c>
-      <c r="W3" t="s">
-        <v>70</v>
-      </c>
-      <c r="X3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>76</v>
       </c>
       <c r="AE3">
         <v>24</v>
       </c>
       <c r="AF3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AN3" t="s">
         <v>97</v>
       </c>
-      <c r="AG3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>70</v>
-      </c>
       <c r="AO3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AP3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AQ3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AR3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AS3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AT3">
         <v>0</v>
       </c>
       <c r="AU3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AV3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AW3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AX3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AY3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AZ3" t="s">
+        <v>98</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB3">
+        <v>56981585232</v>
+      </c>
+      <c r="BC3" t="s">
         <v>100</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BD3" t="s">
         <v>101</v>
       </c>
-      <c r="BB3">
-        <v>977060355</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>102</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>89</v>
-      </c>
       <c r="BE3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BF3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BG3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>43528</v>
+        <v>43567</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>63</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>64</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>65</v>
       </c>
-      <c r="I4" t="s">
-        <v>66</v>
-      </c>
       <c r="J4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" t="s">
+        <v>68</v>
+      </c>
+      <c r="S4" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" t="s">
+        <v>102</v>
+      </c>
+      <c r="U4" t="s">
+        <v>68</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K4" t="s">
-        <v>104</v>
-      </c>
-      <c r="L4" t="s">
-        <v>69</v>
-      </c>
-      <c r="M4" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" t="s">
-        <v>70</v>
-      </c>
-      <c r="P4" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>70</v>
-      </c>
-      <c r="R4" t="s">
-        <v>70</v>
-      </c>
-      <c r="S4" t="s">
-        <v>71</v>
-      </c>
-      <c r="T4" t="s">
-        <v>105</v>
-      </c>
-      <c r="U4" t="s">
-        <v>70</v>
-      </c>
-      <c r="V4" t="s">
-        <v>106</v>
-      </c>
       <c r="W4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="X4" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4">
         <v>2</v>
       </c>
       <c r="AA4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="AB4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD4" t="s">
         <v>70</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>76</v>
       </c>
       <c r="AE4">
         <v>24</v>
       </c>
       <c r="AF4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AG4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AH4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AI4" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="AJ4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AK4" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="AL4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>119</v>
+        <v>71</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="AN4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AO4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AP4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AQ4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AR4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AS4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AT4">
         <v>0</v>
       </c>
       <c r="AU4" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="AV4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AW4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AX4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AY4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AZ4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="BA4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="BB4">
-        <v>934118075</v>
+        <v>955882893</v>
       </c>
       <c r="BC4" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="BD4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="BE4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BF4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BG4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>43527</v>
+        <v>43094</v>
       </c>
       <c r="B5" t="s">
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
         <v>62</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>63</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>64</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>65</v>
       </c>
-      <c r="I5" t="s">
-        <v>66</v>
-      </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="L5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>68</v>
+      </c>
+      <c r="R5" t="s">
+        <v>68</v>
+      </c>
+      <c r="S5" t="s">
         <v>69</v>
       </c>
-      <c r="M5" t="s">
-        <v>70</v>
-      </c>
-      <c r="N5" t="s">
-        <v>70</v>
-      </c>
-      <c r="O5" t="s">
-        <v>70</v>
-      </c>
-      <c r="P5" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>70</v>
-      </c>
-      <c r="R5" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" t="s">
-        <v>71</v>
-      </c>
       <c r="T5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="W5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="X5" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -2133,107 +2231,374 @@
         <v>2</v>
       </c>
       <c r="AA5" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="AB5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" t="s">
         <v>70</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>76</v>
       </c>
       <c r="AE5">
         <v>24</v>
       </c>
       <c r="AF5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AG5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="AH5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AI5" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="AJ5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AK5" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="AL5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>119</v>
+        <v>71</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="AN5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AO5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AP5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AQ5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AR5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AS5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AT5">
         <v>0</v>
       </c>
       <c r="AU5" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="AV5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AW5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AX5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AY5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AZ5" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="BA5" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="BB5">
-        <v>934118075</v>
+        <v>56971869734</v>
       </c>
       <c r="BC5" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="BD5" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="BE5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BF5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="BG5" t="s">
-        <v>70</v>
-      </c>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V7" s="1"/>
+    </row>
+    <row r="8" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V8" s="1"/>
+    </row>
+    <row r="9" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V9" s="1"/>
+    </row>
+    <row r="10" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V10" s="1"/>
+    </row>
+    <row r="11" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V11" s="1"/>
+    </row>
+    <row r="12" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V12" s="1"/>
+    </row>
+    <row r="13" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V22" s="1"/>
+    </row>
+    <row r="38" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V38" s="1"/>
+      <c r="AA38" s="1"/>
+    </row>
+    <row r="42" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="X42" s="1"/>
+      <c r="AA42" s="1"/>
+    </row>
+    <row r="43" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V43" s="1"/>
+      <c r="X43" s="1"/>
+    </row>
+    <row r="44" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V44" s="1"/>
+      <c r="X44" s="1"/>
+    </row>
+    <row r="45" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V45" s="1"/>
+    </row>
+    <row r="46" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V46" s="1"/>
+      <c r="X46" s="1"/>
+    </row>
+    <row r="47" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V47" s="1"/>
+      <c r="X47" s="1"/>
+    </row>
+    <row r="48" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V48" s="1"/>
+      <c r="X48" s="1"/>
+    </row>
+    <row r="49" spans="22:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="X49" s="1"/>
+    </row>
+    <row r="50" spans="22:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+    </row>
+    <row r="51" spans="22:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+    </row>
+    <row r="52" spans="22:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V52" s="1"/>
+    </row>
+    <row r="66" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V66" s="1"/>
+      <c r="AA66" s="1"/>
+    </row>
+    <row r="73" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+    </row>
+    <row r="74" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+    </row>
+    <row r="75" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+    </row>
+    <row r="76" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+    </row>
+    <row r="77" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="X77" s="1"/>
+    </row>
+    <row r="78" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W78" s="1"/>
+    </row>
+    <row r="79" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W79" s="1"/>
+    </row>
+    <row r="80" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W80" s="1"/>
+    </row>
+    <row r="81" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W81" s="1"/>
+    </row>
+    <row r="82" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W82" s="1"/>
+    </row>
+    <row r="83" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W83" s="1"/>
+    </row>
+    <row r="84" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W84" s="1"/>
+    </row>
+    <row r="85" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W85" s="1"/>
+    </row>
+    <row r="86" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W86" s="1"/>
+    </row>
+    <row r="87" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W87" s="1"/>
+    </row>
+    <row r="88" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W88" s="1"/>
+    </row>
+    <row r="89" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W89" s="1"/>
+    </row>
+    <row r="90" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W90" s="1"/>
+    </row>
+    <row r="91" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W91" s="1"/>
+    </row>
+    <row r="92" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W92" s="1"/>
+    </row>
+    <row r="93" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W93" s="1"/>
+    </row>
+    <row r="94" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W94" s="1"/>
+    </row>
+    <row r="95" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W95" s="1"/>
+    </row>
+    <row r="96" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W96" s="1"/>
+    </row>
+    <row r="97" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W97" s="1"/>
+    </row>
+    <row r="98" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W98" s="1"/>
+    </row>
+    <row r="99" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W99" s="1"/>
+    </row>
+    <row r="100" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W100" s="1"/>
+    </row>
+    <row r="101" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W101" s="1"/>
+    </row>
+    <row r="102" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W102" s="1"/>
+    </row>
+    <row r="103" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W103" s="1"/>
+    </row>
+    <row r="104" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W104" s="1"/>
+    </row>
+    <row r="105" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W105" s="1"/>
+    </row>
+    <row r="106" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W106" s="1"/>
+    </row>
+    <row r="107" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W107" s="1"/>
+    </row>
+    <row r="108" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W108" s="1"/>
+    </row>
+    <row r="109" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W109" s="1"/>
+    </row>
+    <row r="110" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W110" s="1"/>
+    </row>
+    <row r="111" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W111" s="1"/>
+    </row>
+    <row r="112" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W112" s="1"/>
+    </row>
+    <row r="113" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W113" s="1"/>
+    </row>
+    <row r="114" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W114" s="1"/>
+    </row>
+    <row r="115" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W115" s="1"/>
+    </row>
+    <row r="116" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W116" s="1"/>
+    </row>
+    <row r="117" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W117" s="1"/>
+    </row>
+    <row r="118" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W118" s="1"/>
+    </row>
+    <row r="119" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W119" s="1"/>
+    </row>
+    <row r="120" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W120" s="1"/>
+    </row>
+    <row r="121" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W121" s="1"/>
+    </row>
+    <row r="122" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W122" s="1"/>
+    </row>
+    <row r="123" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W123" s="1"/>
+    </row>
+    <row r="124" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W124" s="1"/>
+    </row>
+    <row r="125" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W125" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BG5" xr:uid="{B432B93C-6FCD-4719-AF7A-CBEF1073223D}"/>
+  <autoFilter ref="A1:BG125" xr:uid="{EE9B5D47-907A-40D6-BA1C-6246DAD5644F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BG125">
+      <sortCondition sortBy="cellColor" ref="AM1:AM125" dxfId="1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: Restore User.expenses relationship (Fixes Server Startup Crash)
</commit_message>
<xml_diff>
--- a/backend/Coordinados (11).xlsx
+++ b/backend/Coordinados (11).xlsx
@@ -1023,15 +1023,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1373,7 +1365,7 @@
   <dimension ref="A1:BG125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2596,7 +2588,7 @@
   </sheetData>
   <autoFilter ref="A1:BG125" xr:uid="{EE9B5D47-907A-40D6-BA1C-6246DAD5644F}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BG125">
-      <sortCondition sortBy="cellColor" ref="AM1:AM125" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="AM1:AM125" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: Dockerfile usa puerto dinamico PORT para Railway
</commit_message>
<xml_diff>
--- a/backend/Coordinados (11).xlsx
+++ b/backend/Coordinados (11).xlsx
@@ -8,22 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B9A4848-D422-41D1-9E87-175B5229ACE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5964B17B-AD0F-4A35-81DE-65CBD6E541E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{132236D4-E3B4-4A87-BB26-8ED1548DC6E4}"/>
+    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{63507B95-F4E2-41F6-AAFE-C932CA5EB4D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coordinados!$A$1:$BG$125</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="89">
   <si>
     <t>ID</t>
   </si>
@@ -208,6 +205,9 @@
     <t>Sergio Ortiz</t>
   </si>
   <si>
+    <t>Carlos Ruiz</t>
+  </si>
+  <si>
     <t>normal</t>
   </si>
   <si>
@@ -235,254 +235,68 @@
     <t>público</t>
   </si>
   <si>
+    <t>MAIPU- INSTALACIÓN - LUREYE - GENERADOR_SANTIAGO_7</t>
+  </si>
+  <si>
+    <t>Actividad: Instalación 
+Accesorios: GPS 
+Subcuenta de visualización: FLOTA_LUREYE 
+Marca: Sin información 
+Modelo: Sin información 
+Año: Sin informacion</t>
+  </si>
+  <si>
+    <t>Obs I+D: Favor indicar IMEI del dispositivo y nombre que se le colocó</t>
+  </si>
+  <si>
+    <t>Validación KAM: 
+1. actualizar IMEI y nombre en archivo 
+2. Incluir en carpeta respectiva 
+3. formalizar actividad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Soledad Brito 30-12-2025 18:16
+COORDINADO PARA 31.12.25 
+</t>
+  </si>
+  <si>
     <t>NO</t>
   </si>
   <si>
+    <t>LUREYE</t>
+  </si>
+  <si>
+    <t>77030540-3</t>
+  </si>
+  <si>
+    <t>GENERADOR_SANTIAGO_7</t>
+  </si>
+  <si>
     <t>GV310LAU</t>
   </si>
   <si>
+    <t>xaviera.gatica@lureye.cl</t>
+  </si>
+  <si>
+    <t>XAVIERA GATICA</t>
+  </si>
+  <si>
+    <t>AV. LO ESPEJO 1300, MAIPU</t>
+  </si>
+  <si>
+    <t>MAIPU</t>
+  </si>
+  <si>
     <t>Región Metropolitana de Santiago.</t>
   </si>
   <si>
-    <t>Soporte</t>
-  </si>
-  <si>
-    <t>24-12-2025</t>
-  </si>
-  <si>
-    <t>TEMUCO</t>
-  </si>
-  <si>
-    <t>Región de La Araucanía.</t>
-  </si>
-  <si>
-    <t>Arriendo</t>
-  </si>
-  <si>
-    <t>Camión</t>
-  </si>
-  <si>
-    <t>TEMUCO - INSTALACIÓN GPS + ACCESORIOS - DIWATTS - TRPT29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad: Instalación 
-Accesorios: GPS, Corte de motor, Sonda de temperatura y Sensor de puertas  
-Subcuenta de visualización: WATTS2 
-Marca: Hino 
-Modelo: XZU 917 
-Año: 2025 
-Obs: Favor coordinar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 30-12-2025 16:57
-COORDINADO CON MAGDALENA PONCE, PARA 05.01.25
-=-=
-@Soledad Brito 30-12-2025 16:05
-MAGDALENA PONCE, REVISARÁ RUTA Y DEVOLVERÁ EL LLAMADO
-</t>
-  </si>
-  <si>
-    <t>DIWATTS</t>
-  </si>
-  <si>
-    <t>76455830-8</t>
-  </si>
-  <si>
-    <t>TRPT29</t>
-  </si>
-  <si>
-    <t>magdalena.ponce@watts.cl</t>
-  </si>
-  <si>
-    <t>MAGDALENA PONCE</t>
-  </si>
-  <si>
-    <t>PANAMERICANA SUR KM. 678 PADRE LAS CASAS</t>
-  </si>
-  <si>
-    <t>Blanca Acuña</t>
-  </si>
-  <si>
-    <t>27-11-2025</t>
-  </si>
-  <si>
-    <t>CHILLAN - INSTALACIÓN GPS - ACCESORIOS - CIAL_ALIMENTOS - VE839-POR CONFIRMAR</t>
-  </si>
-  <si>
-    <t>ACTIVIDAD: INSTALACIÓN  
-GPS  
-BOTON EMERGENCIA  
-CORTE MOTOR  
-SENSOR DE TEMPERATURA CON DOBLE SONDA 
-2 SENSOR MAGNETICO 
-RETIRO EQUIPO COMPETENCIA  
-Información vehicular 
-VEHICULO NUEVO DISPONIBLE A PARTIR DE LA SEMANA 08/12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDACIÓN I+D  
-1.- VALIDAR POSICION DE DISPOSITIVO GPS  
-2.- VALIDACIÓN DE FUNCIONAMIENTO BOTON EMERGENCIA  
-3.- VALIDACIÓN DE FUNCIONAMIENTO CORTE MOTOR  
-4.- VALIDACIÓN DE FUNCIONAMIENTO SENSOR PUERTA  
-5.- VALIDACIÓN DE SENSOR DE TEMPERATURA (AMBAS SONDAS DEBEN ESTAR FUNCIONALES) 
-6.- FOTOGRAFIA DE GPS COMPETENCIA (NUMERO DE SERIE)  
-7.- FOTOGRAFÍA FISICA DE LA UBICACIÓN DEL GPS (DONDE QUEDA INSTALADO) (OBLIGATORIO) 
-8.- FOTOGRAFÍA DE PATENTE INTERVENIDA  
-9.- OT FIRMADA  
-10.- DAR VISUALIZACIÓN A SUBCUENTA FLOTA_CIALALIMENTOS 
-ZONA Y ALARMA  
-1.- VELOCIDAD 95 KM POR 1 MINUTO  
-2.- CARGA DE ZONAS POR ACCESORIOS IMPLEMENTADOS  
-3.- CARGAR ALARMA DE TEMPERATURA PEGADA  
-4.- SIN COBERTURA GPS  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 30-12-2025 16:55
-RECOORDINADO CON HECTOR CORREA, PARA 08-01-25 A LAS 15:00 HRS
-=-=
-@Blanca Acuña 30-12-2025 16:39
-Estimados favor proceder con coordinación, cliente cuenta con unidad disponible
-=-=
-@Soledad Brito 15-12-2025 10:33
-COORDINADO CON HECTOR CORREA, PARA 18.12.25 A LAS 14:00 HRS.
-=-=
-@Soledad Brito 09-12-2025 17:22
-HECTOR CORREA, CONFIRMARÁ SI PODEMOS REALIZAR LA INSTALACIÓN 10.12.25,
-=-=
-@Nicolas del Rio 05-12-2025 13:21
-ESTIMADOS 
-JUNTO CON SALUDAR. 
-CLIENTE SEÑALA QUE HAY QUE LLAMARLO SEMANA DEL 8 DICIEMBRE PARA VER SI ESTA DISPONIBLE EL NUEVO VEHICULO. 
-GRACIAS 
-SALUDOS
-=-=
-@Nicolas del Rio 03-12-2025 17:40
-ESTIMADAS/OS 
-JUNTO CON SALUDAR, VEHICULO PENDIENTE DE CONFIRMACION POR JO CIAL CHILLAN. 
-FAVOR CUANDO ESTE OK LA SOLICITUD DEL CLIENTE, ENTREGAR A OPERACIONES PARA COORDINAR. 
-QUEDO ATENTO A DUDAS. 
-SALUDOS
-=-=
-@Soledad Brito 01-12-2025 10:27
-COORDINADO PARA 01.12.25 A LAS 13:00 HRS.
-=-=
-@Soledad Brito 28-11-2025 18:08
-HECTOR CORREA INDICA QUE DEVOLVERÁ EL LLAMADO
-=-=
-@Blanca Acuña 27-11-2025 17:03
-Estimada este es el nuevo TKT ya que se mantiene numero interno
-=-=
-@Soledad Brito 27-11-2025 15:47
-POR FAVOR REVISAR QUE PATENTE INSTALARAN EN LUGAR DE ESTA
-</t>
-  </si>
-  <si>
-    <t>CIAL_ALIMENTOS</t>
-  </si>
-  <si>
-    <t>80186300-0</t>
-  </si>
-  <si>
-    <t>VE839-POR CONFIRMAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalación </t>
-  </si>
-  <si>
-    <t>HECTOR CORREA</t>
-  </si>
-  <si>
-    <t>RUTA 5 SUR KM 8 SN</t>
-  </si>
-  <si>
-    <t>CHILLAN</t>
-  </si>
-  <si>
-    <t>Región del Ñuble.</t>
-  </si>
-  <si>
-    <t>SAN BERNARDO - REVISIÓN GPS - CUENTA_CAROZZIDISTRIBUCION - HLPX63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad: Revisión 
-Accesorios: GPS  
-Año GPS: GV310LAU 2024 
-Marca: Sinotruck 
-Modelo: TR 420 
-Año: 2016 
-Obs: Revisar, presenta exceso de saltos de posición. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 30-12-2025 16:49
-COORDINADO CON CHRISTOPHER AGURTO PARA 31.12.25 A LAS 10:00 HRS
-=-=
-@Soledad Brito 30-12-2025 10:52
-CHRISTOPHER AGURTO, REVISARÁ RUTA Y DEVOLVERÁ EL LLAMADO
-</t>
-  </si>
-  <si>
-    <t>CUENTA_CAROZZIDISTRIBUCION</t>
-  </si>
-  <si>
-    <t>96591040-9</t>
-  </si>
-  <si>
-    <t>46406</t>
-  </si>
-  <si>
-    <t>HLPX63</t>
-  </si>
-  <si>
-    <t>christopher.agurto@carozzi.cl</t>
-  </si>
-  <si>
-    <t>CHRISTOPHER AGURTO</t>
-  </si>
-  <si>
-    <t>CAMINO LONGITUDINAL SUR 5201, NOS</t>
-  </si>
-  <si>
-    <t>SAN BERNARDO</t>
-  </si>
-  <si>
-    <t>TEMUCO - CAMBIO GPS + VALIDACIÓN - CUENTA_CAROZZIDISTRIBUCION - BWYY79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVIDAD: CAMBIO GPS +VALIDACIÓN ENTEL </t>
-  </si>
-  <si>
-    <t xml:space="preserve">@Soledad Brito 30-12-2025 13:01
-PEDRO BUSTAMANTE, CELULAR CORRECTO ES +56971869734 X FAVOAR EDITAR, COORDINADO PARA 10.01.26 A LAS 09:00 
-=-=
-@Soledad Brito 30-12-2025 12:55
-PEDRO BUSTAMANTE, INDICA QUE ESTÁN CON MUCHO TRABAJO, QUE TIENEN DISPONIBILIDAD PARA DÍA SABADO 10.01.25 A LAS 09:00 SE ENVIA CORREO CON PROGRAMACIÓN
-</t>
-  </si>
-  <si>
-    <t>19331</t>
-  </si>
-  <si>
-    <t>BWYY79</t>
-  </si>
-  <si>
-    <t>pedro.bustamante@carozzi.cl</t>
-  </si>
-  <si>
-    <t>PEDRO BUSTAMANTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUIDO BECK DE RAMBERGA 1884, PADRE DE LAS CASAS </t>
+    <t>MAIPU- INSTALACIÓN - LUREYE - GENERADOR_SANTIAGO_6</t>
+  </si>
+  <si>
+    <t>GENERADOR_SANTIAGO_6</t>
   </si>
   <si>
     <t>GPS</t>
-  </si>
-  <si>
-    <t>GPS, Corta Corriente, Sensor Pta, Sensor Temperatura</t>
-  </si>
-  <si>
-    <t>GPS, Botón Alámbrico Tablero, Corta Corriente, Sensor Pta, Sensor Pta Adicional, Sensor Temperatura, Sensor Temperatura Adicional</t>
   </si>
 </sst>
 </file>
@@ -625,7 +439,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -803,12 +617,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -972,12 +780,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1023,16 +827,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1361,73 +1156,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9B5D47-907A-40D6-BA1C-6246DAD5644F}">
-  <dimension ref="A1:BG125"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC3348F-0522-48AF-B8EF-6FA5A3FB4A42}">
+  <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.06640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.9296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.06640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="114.53125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="255.59765625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="255.59765625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.06640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.53125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.06640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="109.1328125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="19.796875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.86328125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="36.06640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="50.9296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="21.86328125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="22.19921875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="59.53125" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="15.06640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="41.73046875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="30.46484375" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.53125" customWidth="1"/>
+    <col min="25" max="26" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1606,9 +1351,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>43572</v>
+        <v>43585</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
@@ -1617,980 +1362,354 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K2" t="s">
-        <v>67</v>
-      </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="U2" t="s">
-        <v>68</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
+      </c>
+      <c r="V2" t="s">
+        <v>72</v>
       </c>
       <c r="W2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="X2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AB2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AC2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="AE2">
         <v>24</v>
       </c>
       <c r="AF2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="AG2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="AH2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="AI2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AJ2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="AK2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AL2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>122</v>
+        <v>80</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>88</v>
       </c>
       <c r="AN2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AO2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AP2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AQ2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AR2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AS2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AT2">
         <v>0</v>
       </c>
       <c r="AU2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BB2">
+        <v>978263964</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD2" t="s">
         <v>85</v>
       </c>
-      <c r="AV2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>86</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BB2">
-        <v>972173626</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>75</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>76</v>
-      </c>
       <c r="BE2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BF2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BG2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>42426</v>
+        <v>43584</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
         <v>68</v>
       </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" t="s">
-        <v>89</v>
-      </c>
       <c r="L3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="U3" t="s">
-        <v>68</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
+      </c>
+      <c r="V3" t="s">
+        <v>72</v>
+      </c>
+      <c r="W3" t="s">
+        <v>73</v>
       </c>
       <c r="X3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
         <v>1</v>
       </c>
-      <c r="Z3">
-        <v>10</v>
-      </c>
       <c r="AA3" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="AB3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AC3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="AE3">
         <v>24</v>
       </c>
       <c r="AF3" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="AG3" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="AH3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="AI3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AJ3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="AK3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="AL3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>123</v>
+        <v>80</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>88</v>
       </c>
       <c r="AN3" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="AO3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AP3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AQ3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AR3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AS3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AT3">
         <v>0</v>
       </c>
       <c r="AU3" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="AV3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AW3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AX3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AY3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AZ3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="BA3" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="BB3">
-        <v>56981585232</v>
+        <v>978263964</v>
       </c>
       <c r="BC3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="BD3" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="BE3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BF3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BG3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>43567</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" t="s">
-        <v>68</v>
-      </c>
-      <c r="O4" t="s">
-        <v>68</v>
-      </c>
-      <c r="P4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>68</v>
-      </c>
-      <c r="R4" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" t="s">
-        <v>102</v>
-      </c>
-      <c r="U4" t="s">
-        <v>68</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="W4" t="s">
-        <v>68</v>
-      </c>
-      <c r="X4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y4">
-        <v>1</v>
-      </c>
-      <c r="Z4">
-        <v>2</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE4">
-        <v>24</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>110</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>111</v>
-      </c>
-      <c r="BB4">
-        <v>955882893</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>112</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>43094</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" t="s">
-        <v>73</v>
-      </c>
-      <c r="K5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" t="s">
-        <v>67</v>
-      </c>
-      <c r="M5" t="s">
-        <v>68</v>
-      </c>
-      <c r="N5" t="s">
-        <v>68</v>
-      </c>
-      <c r="O5" t="s">
-        <v>68</v>
-      </c>
-      <c r="P5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>68</v>
-      </c>
-      <c r="R5" t="s">
-        <v>68</v>
-      </c>
-      <c r="S5" t="s">
-        <v>69</v>
-      </c>
-      <c r="T5" t="s">
-        <v>113</v>
-      </c>
-      <c r="U5" t="s">
-        <v>68</v>
-      </c>
-      <c r="V5" t="s">
-        <v>114</v>
-      </c>
-      <c r="W5" t="s">
-        <v>68</v>
-      </c>
-      <c r="X5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>2</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE5">
-        <v>24</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>118</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>119</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB5">
-        <v>56971869734</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>75</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>76</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>68</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>68</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V6" s="1"/>
-    </row>
-    <row r="7" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V12" s="1"/>
-    </row>
-    <row r="13" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V13" s="1"/>
-    </row>
-    <row r="14" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V14" s="1"/>
-    </row>
-    <row r="15" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="1:59" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V20" s="1"/>
-    </row>
-    <row r="21" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="22:22" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V22" s="1"/>
-    </row>
-    <row r="38" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V38" s="1"/>
-      <c r="AA38" s="1"/>
-    </row>
-    <row r="42" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="X42" s="1"/>
-      <c r="AA42" s="1"/>
-    </row>
-    <row r="43" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V43" s="1"/>
-      <c r="X43" s="1"/>
-    </row>
-    <row r="44" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V44" s="1"/>
-      <c r="X44" s="1"/>
-    </row>
-    <row r="45" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V45" s="1"/>
-    </row>
-    <row r="46" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V46" s="1"/>
-      <c r="X46" s="1"/>
-    </row>
-    <row r="47" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V47" s="1"/>
-      <c r="X47" s="1"/>
-    </row>
-    <row r="48" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V48" s="1"/>
-      <c r="X48" s="1"/>
-    </row>
-    <row r="49" spans="22:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="X49" s="1"/>
-    </row>
-    <row r="50" spans="22:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
-    </row>
-    <row r="51" spans="22:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V51" s="1"/>
-      <c r="W51" s="1"/>
-    </row>
-    <row r="52" spans="22:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V52" s="1"/>
-    </row>
-    <row r="66" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V66" s="1"/>
-      <c r="AA66" s="1"/>
-    </row>
-    <row r="73" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V73" s="1"/>
-      <c r="W73" s="1"/>
-    </row>
-    <row r="74" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V74" s="1"/>
-      <c r="W74" s="1"/>
-    </row>
-    <row r="75" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V75" s="1"/>
-      <c r="W75" s="1"/>
-    </row>
-    <row r="76" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="V76" s="1"/>
-      <c r="W76" s="1"/>
-    </row>
-    <row r="77" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="X77" s="1"/>
-    </row>
-    <row r="78" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W78" s="1"/>
-    </row>
-    <row r="79" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W79" s="1"/>
-    </row>
-    <row r="80" spans="22:27" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W80" s="1"/>
-    </row>
-    <row r="81" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W81" s="1"/>
-    </row>
-    <row r="82" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W82" s="1"/>
-    </row>
-    <row r="83" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W83" s="1"/>
-    </row>
-    <row r="84" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W84" s="1"/>
-    </row>
-    <row r="85" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W85" s="1"/>
-    </row>
-    <row r="86" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W86" s="1"/>
-    </row>
-    <row r="87" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W87" s="1"/>
-    </row>
-    <row r="88" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W88" s="1"/>
-    </row>
-    <row r="89" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W89" s="1"/>
-    </row>
-    <row r="90" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W90" s="1"/>
-    </row>
-    <row r="91" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W91" s="1"/>
-    </row>
-    <row r="92" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W92" s="1"/>
-    </row>
-    <row r="93" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W93" s="1"/>
-    </row>
-    <row r="94" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W94" s="1"/>
-    </row>
-    <row r="95" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W95" s="1"/>
-    </row>
-    <row r="96" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W96" s="1"/>
-    </row>
-    <row r="97" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W97" s="1"/>
-    </row>
-    <row r="98" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W98" s="1"/>
-    </row>
-    <row r="99" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W99" s="1"/>
-    </row>
-    <row r="100" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W100" s="1"/>
-    </row>
-    <row r="101" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W101" s="1"/>
-    </row>
-    <row r="102" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W102" s="1"/>
-    </row>
-    <row r="103" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W103" s="1"/>
-    </row>
-    <row r="104" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W104" s="1"/>
-    </row>
-    <row r="105" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W105" s="1"/>
-    </row>
-    <row r="106" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W106" s="1"/>
-    </row>
-    <row r="107" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W107" s="1"/>
-    </row>
-    <row r="108" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W108" s="1"/>
-    </row>
-    <row r="109" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W109" s="1"/>
-    </row>
-    <row r="110" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W110" s="1"/>
-    </row>
-    <row r="111" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W111" s="1"/>
-    </row>
-    <row r="112" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W112" s="1"/>
-    </row>
-    <row r="113" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W113" s="1"/>
-    </row>
-    <row r="114" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W114" s="1"/>
-    </row>
-    <row r="115" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W115" s="1"/>
-    </row>
-    <row r="116" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W116" s="1"/>
-    </row>
-    <row r="117" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W117" s="1"/>
-    </row>
-    <row r="118" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W118" s="1"/>
-    </row>
-    <row r="119" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W119" s="1"/>
-    </row>
-    <row r="120" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W120" s="1"/>
-    </row>
-    <row r="121" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W121" s="1"/>
-    </row>
-    <row r="122" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W122" s="1"/>
-    </row>
-    <row r="123" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W123" s="1"/>
-    </row>
-    <row r="124" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W124" s="1"/>
-    </row>
-    <row r="125" spans="23:23" ht="13.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="W125" s="1"/>
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BG125" xr:uid="{EE9B5D47-907A-40D6-BA1C-6246DAD5644F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BG125">
-      <sortCondition sortBy="cellColor" ref="AM1:AM125" dxfId="0"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>